<commit_message>
Updating GBR status + adding README.md
</commit_message>
<xml_diff>
--- a/cfg/CPC_CONFIGURATIONS.xlsx
+++ b/cfg/CPC_CONFIGURATIONS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\IOTC working parties\iotc-tcac-simulations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\IOTC working parties\iotc-tcac-simulations\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24E6931-CEA9-47E2-887F-11C72853DD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8F28CE-8BCB-4593-A1F3-93975894459D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
+    <workbookView xWindow="28680" yWindow="1140" windowWidth="29040" windowHeight="15720" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
   </bookViews>
   <sheets>
     <sheet name="CPC" sheetId="1" r:id="rId1"/>
@@ -243,9 +243,6 @@
     <t>COASTAL</t>
   </si>
   <si>
-    <t>EEZ_SIZE</t>
-  </si>
-  <si>
     <t>PER_CAPITA_FISH_CONSUMPTION_KG</t>
   </si>
   <si>
@@ -297,10 +294,37 @@
     <t>SQL query</t>
   </si>
   <si>
-    <t>EEZ_IOTC_RELATIVE_SIZE</t>
-  </si>
-  <si>
-    <t>AUNJ_AREA</t>
+    <t xml:space="preserve">GNI status </t>
+  </si>
+  <si>
+    <t>Development status</t>
+  </si>
+  <si>
+    <t>https://www.un.org/development/desa/dpad/wp-content/uploads/sites/45/WESP2020_Annex.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - For the EU averaged from:</t>
+  </si>
+  <si>
+    <t>https://www.theglobaleconomy.com/rankings/human_development/European-union/</t>
+  </si>
+  <si>
+    <t>https://datahelpdesk.worldbank.org/knowledgebase/articles/906519-world-bank-country-and-lending-group</t>
+  </si>
+  <si>
+    <t>PROP_WORKERS_EMPLOYED_SSF</t>
+  </si>
+  <si>
+    <t>PROP_FISHERIES_CONTRIBUTION_GDP</t>
+  </si>
+  <si>
+    <t>PROP_EXPORT_VALUE_FISHERY</t>
+  </si>
+  <si>
+    <t>Dummy values, waiting for actual values to be provided by the proponents</t>
+  </si>
+  <si>
+    <t>HAS_NJA_IO</t>
   </si>
   <si>
     <t>USE [IOTC_master]
@@ -313,7 +337,7 @@
     C.NAME_EN,
     CASE WHEN H.CONTRACTING_PARTY = 1 THEN 'CPC' ELSE 'CNCP' END AS [STATUS],
     CASE WHEN C.CODE = 'EUR' THEN 0 ELSE C.IS_COASTAL END AS COASTAL, 
-    C.IS_COASTAL AS AUNJ_AREA,
+    C.IS_COASTAL AS HAS_NJA_IO,
     C.IS_SIDS AS SIDS,
     COALESCE(
         CASE 
@@ -321,14 +345,14 @@
             ELSE A.OCEAN_AREA_IOTC_KM2 
         END, 
         ''
-    ) AS EEZ_SIZE, 
+    ) AS NJA_SIZE, 
     COALESCE(
         CASE 
             WHEN C.CODE = 'GBR' THEN ROUND(@CHAGOS_AREA / @IOTC_AREA, 4)
             ELSE ROUND(A.OCEAN_AREA_IO_KM2 / @IOTC_AREA, 4) 
         END, 
         ''
-    ) AS EEZ_IOTC_RELATIVE_SIZE
+    ) AS NJA_IOTC_RELATIVE_SIZE
 FROM 
     [IOTC_master].[refs_admin].[CPCS] C
 INNER JOIN
@@ -345,34 +369,10 @@
     1 ASC</t>
   </si>
   <si>
-    <t xml:space="preserve">GNI status </t>
-  </si>
-  <si>
-    <t>Development status</t>
-  </si>
-  <si>
-    <t>https://www.un.org/development/desa/dpad/wp-content/uploads/sites/45/WESP2020_Annex.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - For the EU averaged from:</t>
-  </si>
-  <si>
-    <t>https://www.theglobaleconomy.com/rankings/human_development/European-union/</t>
-  </si>
-  <si>
-    <t>https://datahelpdesk.worldbank.org/knowledgebase/articles/906519-world-bank-country-and-lending-group</t>
-  </si>
-  <si>
-    <t>PROP_WORKERS_EMPLOYED_SSF</t>
-  </si>
-  <si>
-    <t>PROP_FISHERIES_CONTRIBUTION_GDP</t>
-  </si>
-  <si>
-    <t>PROP_EXPORT_VALUE_FISHERY</t>
-  </si>
-  <si>
-    <t>Dummy values, waiting for actual values to be provided by the proponents</t>
+    <t>NJA_SIZE</t>
+  </si>
+  <si>
+    <t>NJA_IOTC_RELATIVE_SIZE</t>
   </si>
 </sst>
 </file>
@@ -463,15 +463,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -797,9 +797,9 @@
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.28515625" customWidth="1"/>
@@ -816,36 +816,36 @@
         <v>65</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>86</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
+        <v>97</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -858,13 +858,13 @@
         <v>63</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>4320207</v>
@@ -872,21 +872,21 @@
       <c r="H2" s="2">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="J2" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
+      <c r="J2" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
@@ -903,13 +903,13 @@
         <v>63</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>77773</v>
@@ -917,19 +917,19 @@
       <c r="H3" s="2">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
@@ -960,19 +960,19 @@
       <c r="H4" s="2">
         <v>0</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13"/>
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
@@ -1003,19 +1003,19 @@
       <c r="H5" s="2">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
@@ -1035,10 +1035,10 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>378244</v>
@@ -1046,19 +1046,19 @@
       <c r="H6" s="2">
         <v>6.1000000000000004E-3</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
       <c r="W6" s="5"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
@@ -1075,13 +1075,13 @@
         <v>63</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>1294307</v>
@@ -1089,19 +1089,19 @@
       <c r="H7" s="2">
         <v>3.6900000000000002E-2</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
       <c r="W7" s="5"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
@@ -1121,10 +1121,10 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>638580</v>
@@ -1132,19 +1132,19 @@
       <c r="H8" s="2">
         <v>1.04E-2</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
       <c r="W8" s="5"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
@@ -1161,13 +1161,13 @@
         <v>63</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>1948313</v>
@@ -1175,19 +1175,19 @@
       <c r="H9" s="2">
         <v>3.1600000000000003E-2</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
       <c r="W9" s="5"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>
@@ -1204,13 +1204,13 @@
         <v>63</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <v>2283347</v>
@@ -1218,19 +1218,19 @@
       <c r="H10" s="2">
         <v>3.7100000000000001E-2</v>
       </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
@@ -1247,13 +1247,13 @@
         <v>63</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>161846</v>
@@ -1261,19 +1261,19 @@
       <c r="H11" s="2">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
       <c r="W11" s="5"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="5"/>
@@ -1304,19 +1304,19 @@
       <c r="H12" s="2">
         <v>0</v>
       </c>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
@@ -1333,13 +1333,13 @@
         <v>63</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>111436</v>
@@ -1347,19 +1347,19 @@
       <c r="H13" s="2">
         <v>1.8E-3</v>
       </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
@@ -1390,19 +1390,19 @@
       <c r="H14" s="2">
         <v>0</v>
       </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
       <c r="W14" s="5"/>
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
@@ -1433,19 +1433,19 @@
       <c r="H15" s="2">
         <v>0</v>
       </c>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-      <c r="V15" s="10"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
@@ -1462,13 +1462,13 @@
         <v>63</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
         <v>530275</v>
@@ -1476,19 +1476,19 @@
       <c r="H16" s="2">
         <v>8.6E-3</v>
       </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
       <c r="Y16" s="5"/>
@@ -1505,13 +1505,13 @@
         <v>63</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <v>1199904</v>
@@ -1519,19 +1519,19 @@
       <c r="H17" s="2">
         <v>1.95E-2</v>
       </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
       <c r="W17" s="5"/>
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
@@ -1548,13 +1548,13 @@
         <v>63</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <v>916244</v>
@@ -1562,19 +1562,19 @@
       <c r="H18" s="2">
         <v>1.49E-2</v>
       </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
       <c r="W18" s="5"/>
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
@@ -1591,13 +1591,13 @@
         <v>63</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>570059</v>
@@ -1605,19 +1605,19 @@
       <c r="H19" s="2">
         <v>9.2999999999999992E-3</v>
       </c>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-      <c r="V19" s="10"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
       <c r="W19" s="5"/>
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
@@ -1648,19 +1648,19 @@
       <c r="H20" s="2">
         <v>2.07E-2</v>
       </c>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
       <c r="W20" s="5"/>
       <c r="X20" s="5"/>
       <c r="Y20" s="5"/>
@@ -1677,13 +1677,13 @@
         <v>63</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <v>62343</v>
@@ -1691,19 +1691,19 @@
       <c r="H21" s="2">
         <v>1E-3</v>
       </c>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="10"/>
-      <c r="V21" s="10"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13"/>
       <c r="W21" s="5"/>
       <c r="X21" s="5"/>
       <c r="Y21" s="5"/>
@@ -1720,13 +1720,13 @@
         <v>63</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <v>535212</v>
@@ -1734,19 +1734,19 @@
       <c r="H22" s="2">
         <v>8.6999999999999994E-3</v>
       </c>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
-      <c r="V22" s="10"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13"/>
       <c r="W22" s="5"/>
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
@@ -1763,13 +1763,13 @@
         <v>63</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
         <v>220792</v>
@@ -1777,19 +1777,19 @@
       <c r="H23" s="2">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
       <c r="W23" s="5"/>
       <c r="X23" s="5"/>
       <c r="Y23" s="5"/>
@@ -1820,19 +1820,19 @@
       <c r="H24" s="2">
         <v>0</v>
       </c>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10"/>
-      <c r="T24" s="10"/>
-      <c r="U24" s="10"/>
-      <c r="V24" s="10"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13"/>
       <c r="W24" s="5"/>
       <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
@@ -1849,13 +1849,13 @@
         <v>63</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
         <v>66483</v>
@@ -1863,19 +1863,19 @@
       <c r="H25" s="2">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="10"/>
-      <c r="T25" s="10"/>
-      <c r="U25" s="10"/>
-      <c r="V25" s="10"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="13"/>
       <c r="W25" s="5"/>
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
@@ -1892,13 +1892,13 @@
         <v>63</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <v>829359</v>
@@ -1906,19 +1906,19 @@
       <c r="H26" s="2">
         <v>1.35E-2</v>
       </c>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
-      <c r="S26" s="10"/>
-      <c r="T26" s="10"/>
-      <c r="U26" s="10"/>
-      <c r="V26" s="10"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="13"/>
       <c r="W26" s="5"/>
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
@@ -1949,19 +1949,19 @@
       <c r="H27" s="2">
         <v>2.1600000000000001E-2</v>
       </c>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="10"/>
-      <c r="V27" s="10"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
       <c r="W27" s="5"/>
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
@@ -1978,13 +1978,13 @@
         <v>63</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
         <v>118137</v>
@@ -1992,19 +1992,19 @@
       <c r="H28" s="2">
         <v>1.9E-3</v>
       </c>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
-      <c r="S28" s="10"/>
-      <c r="T28" s="10"/>
-      <c r="U28" s="10"/>
-      <c r="V28" s="10"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="13"/>
       <c r="W28" s="5"/>
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
@@ -2021,13 +2021,13 @@
         <v>63</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
         <v>240763</v>
@@ -2035,19 +2035,19 @@
       <c r="H29" s="2">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
-      <c r="S29" s="10"/>
-      <c r="T29" s="10"/>
-      <c r="U29" s="10"/>
-      <c r="V29" s="10"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="13"/>
       <c r="W29" s="5"/>
       <c r="X29" s="5"/>
       <c r="Y29" s="5"/>
@@ -2064,13 +2064,13 @@
         <v>63</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30">
         <v>543647</v>
@@ -2078,19 +2078,19 @@
       <c r="H30" s="2">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="10"/>
-      <c r="T30" s="10"/>
-      <c r="U30" s="10"/>
-      <c r="V30" s="10"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="13"/>
       <c r="W30" s="5"/>
       <c r="X30" s="5"/>
       <c r="Y30" s="5"/>
@@ -2107,13 +2107,13 @@
         <v>63</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31">
         <v>781573</v>
@@ -2121,282 +2121,282 @@
       <c r="H31" s="2">
         <v>1.89E-2</v>
       </c>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
-      <c r="Q31" s="10"/>
-      <c r="R31" s="10"/>
-      <c r="S31" s="10"/>
-      <c r="T31" s="10"/>
-      <c r="U31" s="10"/>
-      <c r="V31" s="10"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="13"/>
       <c r="W31" s="5"/>
       <c r="X31" s="5"/>
       <c r="Y31" s="5"/>
       <c r="Z31" s="5"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
-      <c r="R32" s="10"/>
-      <c r="S32" s="10"/>
-      <c r="T32" s="10"/>
-      <c r="U32" s="10"/>
-      <c r="V32" s="10"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
       <c r="W32" s="5"/>
       <c r="X32" s="5"/>
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
     </row>
     <row r="33" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="10"/>
-      <c r="T33" s="10"/>
-      <c r="U33" s="10"/>
-      <c r="V33" s="10"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="13"/>
+      <c r="V33" s="13"/>
     </row>
     <row r="34" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
-      <c r="S34" s="10"/>
-      <c r="T34" s="10"/>
-      <c r="U34" s="10"/>
-      <c r="V34" s="10"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="13"/>
     </row>
     <row r="35" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
-      <c r="S35" s="10"/>
-      <c r="T35" s="10"/>
-      <c r="U35" s="10"/>
-      <c r="V35" s="10"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="13"/>
+      <c r="R35" s="13"/>
+      <c r="S35" s="13"/>
+      <c r="T35" s="13"/>
+      <c r="U35" s="13"/>
+      <c r="V35" s="13"/>
     </row>
     <row r="36" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10"/>
-      <c r="S36" s="10"/>
-      <c r="T36" s="10"/>
-      <c r="U36" s="10"/>
-      <c r="V36" s="10"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
     </row>
     <row r="37" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
-      <c r="Q37" s="10"/>
-      <c r="R37" s="10"/>
-      <c r="S37" s="10"/>
-      <c r="T37" s="10"/>
-      <c r="U37" s="10"/>
-      <c r="V37" s="10"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="13"/>
+      <c r="S37" s="13"/>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13"/>
+      <c r="V37" s="13"/>
     </row>
     <row r="38" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="10"/>
-      <c r="S38" s="10"/>
-      <c r="T38" s="10"/>
-      <c r="U38" s="10"/>
-      <c r="V38" s="10"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="13"/>
+      <c r="U38" s="13"/>
+      <c r="V38" s="13"/>
     </row>
     <row r="39" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="10"/>
-      <c r="S39" s="10"/>
-      <c r="T39" s="10"/>
-      <c r="U39" s="10"/>
-      <c r="V39" s="10"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="13"/>
+      <c r="S39" s="13"/>
+      <c r="T39" s="13"/>
+      <c r="U39" s="13"/>
+      <c r="V39" s="13"/>
     </row>
     <row r="40" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="10"/>
-      <c r="R40" s="10"/>
-      <c r="S40" s="10"/>
-      <c r="T40" s="10"/>
-      <c r="U40" s="10"/>
-      <c r="V40" s="10"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="13"/>
+      <c r="P40" s="13"/>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="13"/>
+      <c r="S40" s="13"/>
+      <c r="T40" s="13"/>
+      <c r="U40" s="13"/>
+      <c r="V40" s="13"/>
     </row>
     <row r="41" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
-      <c r="Q41" s="10"/>
-      <c r="R41" s="10"/>
-      <c r="S41" s="10"/>
-      <c r="T41" s="10"/>
-      <c r="U41" s="10"/>
-      <c r="V41" s="10"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13"/>
+      <c r="V41" s="13"/>
     </row>
     <row r="42" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="10"/>
-      <c r="R42" s="10"/>
-      <c r="S42" s="10"/>
-      <c r="T42" s="10"/>
-      <c r="U42" s="10"/>
-      <c r="V42" s="10"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="13"/>
+      <c r="U42" s="13"/>
+      <c r="V42" s="13"/>
     </row>
     <row r="43" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="10"/>
-      <c r="R43" s="10"/>
-      <c r="S43" s="10"/>
-      <c r="T43" s="10"/>
-      <c r="U43" s="10"/>
-      <c r="V43" s="10"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13"/>
+      <c r="V43" s="13"/>
     </row>
     <row r="44" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J44" s="10"/>
-      <c r="K44" s="10"/>
-      <c r="L44" s="10"/>
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-      <c r="S44" s="10"/>
-      <c r="T44" s="10"/>
-      <c r="U44" s="10"/>
-      <c r="V44" s="10"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="13"/>
+      <c r="P44" s="13"/>
+      <c r="Q44" s="13"/>
+      <c r="R44" s="13"/>
+      <c r="S44" s="13"/>
+      <c r="T44" s="13"/>
+      <c r="U44" s="13"/>
+      <c r="V44" s="13"/>
     </row>
     <row r="45" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J45" s="10"/>
-      <c r="K45" s="10"/>
-      <c r="L45" s="10"/>
-      <c r="M45" s="10"/>
-      <c r="N45" s="10"/>
-      <c r="O45" s="10"/>
-      <c r="P45" s="10"/>
-      <c r="Q45" s="10"/>
-      <c r="R45" s="10"/>
-      <c r="S45" s="10"/>
-      <c r="T45" s="10"/>
-      <c r="U45" s="10"/>
-      <c r="V45" s="10"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="13"/>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="13"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="13"/>
+      <c r="T45" s="13"/>
+      <c r="U45" s="13"/>
+      <c r="V45" s="13"/>
     </row>
     <row r="46" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J46" s="10"/>
-      <c r="K46" s="10"/>
-      <c r="L46" s="10"/>
-      <c r="M46" s="10"/>
-      <c r="N46" s="10"/>
-      <c r="O46" s="10"/>
-      <c r="P46" s="10"/>
-      <c r="Q46" s="10"/>
-      <c r="R46" s="10"/>
-      <c r="S46" s="10"/>
-      <c r="T46" s="10"/>
-      <c r="U46" s="10"/>
-      <c r="V46" s="10"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="13"/>
+      <c r="T46" s="13"/>
+      <c r="U46" s="13"/>
+      <c r="V46" s="13"/>
     </row>
     <row r="47" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J47" s="10"/>
-      <c r="K47" s="10"/>
-      <c r="L47" s="10"/>
-      <c r="M47" s="10"/>
-      <c r="N47" s="10"/>
-      <c r="O47" s="10"/>
-      <c r="P47" s="10"/>
-      <c r="Q47" s="10"/>
-      <c r="R47" s="10"/>
-      <c r="S47" s="10"/>
-      <c r="T47" s="10"/>
-      <c r="U47" s="10"/>
-      <c r="V47" s="10"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="13"/>
+      <c r="R47" s="13"/>
+      <c r="S47" s="13"/>
+      <c r="T47" s="13"/>
+      <c r="U47" s="13"/>
+      <c r="V47" s="13"/>
     </row>
     <row r="48" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
-      <c r="L48" s="10"/>
-      <c r="M48" s="10"/>
-      <c r="N48" s="10"/>
-      <c r="O48" s="10"/>
-      <c r="P48" s="10"/>
-      <c r="Q48" s="10"/>
-      <c r="R48" s="10"/>
-      <c r="S48" s="10"/>
-      <c r="T48" s="10"/>
-      <c r="U48" s="10"/>
-      <c r="V48" s="10"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="13"/>
+      <c r="P48" s="13"/>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="13"/>
+      <c r="S48" s="13"/>
+      <c r="T48" s="13"/>
+      <c r="U48" s="13"/>
+      <c r="V48" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2412,7 +2412,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6A7977-2381-4943-AA16-A4F852F13E83}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2431,28 +2433,28 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>70</v>
-      </c>
-      <c r="I1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2460,29 +2462,29 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="12">
-        <v>1</v>
-      </c>
-      <c r="D2" s="12">
+        <v>73</v>
+      </c>
+      <c r="C2" s="10">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10">
         <v>10</v>
       </c>
-      <c r="E2" s="13">
-        <v>0</v>
-      </c>
-      <c r="F2" s="13">
+      <c r="E2" s="11">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11">
         <f t="shared" ref="F2:F25" si="0">F3+0.01</f>
         <v>0.25000000000000006</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="11">
         <v>0</v>
       </c>
       <c r="H2" s="3">
         <v>0.95099999999999996</v>
       </c>
       <c r="I2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2490,25 +2492,25 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="12">
+        <v>72</v>
+      </c>
+      <c r="C3" s="10">
         <f>C2+1</f>
         <v>2</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="10">
         <f>D2+5</f>
         <v>15</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="11">
         <f>E2+0.01</f>
         <v>0.01</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="11">
         <f t="shared" si="0"/>
         <v>0.24000000000000007</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="11">
         <f>G2+0.01</f>
         <v>0.01</v>
       </c>
@@ -2516,7 +2518,7 @@
         <v>0.66100000000000003</v>
       </c>
       <c r="I3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2524,25 +2526,25 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="12">
-        <f t="shared" ref="C4:C27" si="1">C3+1</f>
+        <v>72</v>
+      </c>
+      <c r="C4" s="10">
+        <f t="shared" ref="C4:C26" si="1">C3+1</f>
         <v>3</v>
       </c>
-      <c r="D4" s="12">
-        <f t="shared" ref="D4:D27" si="2">D3+5</f>
+      <c r="D4" s="10">
+        <f t="shared" ref="D4:D26" si="2">D3+5</f>
         <v>20</v>
       </c>
-      <c r="E4" s="13">
-        <f t="shared" ref="E4:G27" si="3">E3+0.01</f>
+      <c r="E4" s="11">
+        <f t="shared" ref="E4:G26" si="3">E3+0.01</f>
         <v>0.02</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="11">
         <f t="shared" si="0"/>
         <v>0.23000000000000007</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="11">
         <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
@@ -2550,7 +2552,7 @@
         <v>0.55800000000000005</v>
       </c>
       <c r="I4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2558,25 +2560,25 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="12">
+        <v>73</v>
+      </c>
+      <c r="C5" s="10">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="10">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="11">
         <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="11">
         <f t="shared" si="0"/>
         <v>0.22000000000000006</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="11">
         <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
@@ -2584,7 +2586,7 @@
         <v>0.90300000000000002</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2592,25 +2594,25 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="12">
+        <v>74</v>
+      </c>
+      <c r="C6" s="10">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="10">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="11">
         <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="11">
         <f t="shared" si="0"/>
         <v>0.21000000000000005</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="11">
         <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
@@ -2618,7 +2620,7 @@
         <v>0.70499999999999996</v>
       </c>
       <c r="I6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2626,25 +2628,25 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="12">
+        <v>74</v>
+      </c>
+      <c r="C7" s="10">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="10">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="11">
         <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="11">
         <f t="shared" si="0"/>
         <v>0.20000000000000004</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="11">
         <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
@@ -2652,7 +2654,7 @@
         <v>0.63300000000000001</v>
       </c>
       <c r="I7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2660,25 +2662,25 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="12">
+        <v>74</v>
+      </c>
+      <c r="C8" s="10">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="10">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="11">
         <f t="shared" si="3"/>
         <v>6.0000000000000005E-2</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="11">
         <f t="shared" si="0"/>
         <v>0.19000000000000003</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="11">
         <f t="shared" si="3"/>
         <v>6.0000000000000005E-2</v>
       </c>
@@ -2686,7 +2688,7 @@
         <v>0.77400000000000002</v>
       </c>
       <c r="I8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2694,25 +2696,25 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="12">
+        <v>74</v>
+      </c>
+      <c r="C9" s="10">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="10">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="11">
         <f t="shared" si="3"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="11">
         <f t="shared" si="0"/>
         <v>0.18000000000000002</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="11">
         <f t="shared" si="3"/>
         <v>7.0000000000000007E-2</v>
       </c>
@@ -2720,7 +2722,7 @@
         <v>0.57499999999999996</v>
       </c>
       <c r="I9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2728,25 +2730,25 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="12">
+        <v>74</v>
+      </c>
+      <c r="C10" s="10">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="10">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="11">
         <f t="shared" si="3"/>
         <v>0.08</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="11">
         <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="11">
         <f t="shared" si="3"/>
         <v>0.08</v>
       </c>
@@ -2754,7 +2756,7 @@
         <v>0.78200000000000003</v>
       </c>
       <c r="I10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2762,25 +2764,25 @@
         <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="12">
+        <v>72</v>
+      </c>
+      <c r="C11" s="10">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="10">
         <f t="shared" si="2"/>
         <v>55</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="11">
         <f t="shared" si="3"/>
         <v>0.09</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="11">
         <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="11">
         <f t="shared" si="3"/>
         <v>0.09</v>
       </c>
@@ -2788,7 +2790,7 @@
         <v>0.501</v>
       </c>
       <c r="I11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2796,25 +2798,25 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="12">
+        <v>74</v>
+      </c>
+      <c r="C12" s="10">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="10">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="11">
         <f t="shared" si="3"/>
         <v>9.9999999999999992E-2</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="11">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="11">
         <f t="shared" si="3"/>
         <v>9.9999999999999992E-2</v>
       </c>
@@ -2822,7 +2824,7 @@
         <v>0.747</v>
       </c>
       <c r="I12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2830,25 +2832,25 @@
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="12">
+        <v>72</v>
+      </c>
+      <c r="C13" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="10">
         <f t="shared" si="2"/>
         <v>65</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="11">
         <f t="shared" si="3"/>
         <v>0.10999999999999999</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="11">
         <f t="shared" si="0"/>
         <v>0.13999999999999999</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="11">
         <f t="shared" si="3"/>
         <v>0.10999999999999999</v>
       </c>
@@ -2856,7 +2858,7 @@
         <v>0.44600000000000001</v>
       </c>
       <c r="I13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2864,25 +2866,25 @@
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="12">
+        <v>74</v>
+      </c>
+      <c r="C14" s="10">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="10">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="11">
         <f t="shared" si="3"/>
         <v>0.11999999999999998</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="11">
         <f t="shared" si="0"/>
         <v>0.12999999999999998</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="11">
         <f t="shared" si="3"/>
         <v>0.11999999999999998</v>
       </c>
@@ -2890,7 +2892,7 @@
         <v>0.80200000000000005</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2898,25 +2900,25 @@
         <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="12">
+        <v>74</v>
+      </c>
+      <c r="C15" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="10">
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="11">
         <f t="shared" si="3"/>
         <v>0.12999999999999998</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="11">
         <f t="shared" si="0"/>
         <v>0.11999999999999998</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="11">
         <f t="shared" si="3"/>
         <v>0.12999999999999998</v>
       </c>
@@ -2924,7 +2926,7 @@
         <v>0.80300000000000005</v>
       </c>
       <c r="I15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2932,25 +2934,25 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="12">
+        <v>74</v>
+      </c>
+      <c r="C16" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="10">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="11">
         <f t="shared" si="3"/>
         <v>0.13999999999999999</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="11">
         <f t="shared" si="0"/>
         <v>0.10999999999999999</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="11">
         <f t="shared" si="3"/>
         <v>0.13999999999999999</v>
       </c>
@@ -2958,7 +2960,7 @@
         <v>0.81599999999999995</v>
       </c>
       <c r="I16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2966,25 +2968,25 @@
         <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="12">
+        <v>74</v>
+      </c>
+      <c r="C17" s="10">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="10">
         <f t="shared" si="2"/>
         <v>85</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="11">
         <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="11">
         <f t="shared" si="0"/>
         <v>9.9999999999999992E-2</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="11">
         <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
@@ -2992,7 +2994,7 @@
         <v>0.54400000000000004</v>
       </c>
       <c r="I17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3000,25 +3002,25 @@
         <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="12">
+        <v>72</v>
+      </c>
+      <c r="C18" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="10">
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="11">
         <f t="shared" si="3"/>
         <v>0.16</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="11">
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="11">
         <f t="shared" si="3"/>
         <v>0.16</v>
       </c>
@@ -3026,7 +3028,7 @@
         <v>0.50800000000000001</v>
       </c>
       <c r="I18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3034,33 +3036,33 @@
         <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="12">
+        <v>72</v>
+      </c>
+      <c r="C19" s="10">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="10">
         <f t="shared" si="2"/>
         <v>95</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="11">
         <f t="shared" si="3"/>
         <v>0.17</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="11">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="11">
         <f t="shared" si="3"/>
         <v>0.17</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3068,25 +3070,25 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="12">
+        <v>74</v>
+      </c>
+      <c r="C20" s="10">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="10">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="11">
         <f t="shared" si="3"/>
         <v>0.18000000000000002</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="11">
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="11">
         <f t="shared" si="3"/>
         <v>0.18000000000000002</v>
       </c>
@@ -3094,7 +3096,7 @@
         <v>0.78500000000000003</v>
       </c>
       <c r="I20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -3102,25 +3104,25 @@
         <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="12">
+        <v>74</v>
+      </c>
+      <c r="C21" s="10">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="10">
         <f t="shared" si="2"/>
         <v>105</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="11">
         <f t="shared" si="3"/>
         <v>0.19000000000000003</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="11">
         <f t="shared" si="0"/>
         <v>6.0000000000000005E-2</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="11">
         <f t="shared" si="3"/>
         <v>0.19000000000000003</v>
       </c>
@@ -3128,7 +3130,7 @@
         <v>0.8</v>
       </c>
       <c r="I21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3136,25 +3138,25 @@
         <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" s="12">
+        <v>72</v>
+      </c>
+      <c r="C22" s="10">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="10">
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="11">
         <f t="shared" si="3"/>
         <v>0.20000000000000004</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="11">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="11">
         <f t="shared" si="3"/>
         <v>0.20000000000000004</v>
       </c>
@@ -3162,7 +3164,7 @@
         <v>0.54900000000000004</v>
       </c>
       <c r="I22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3170,25 +3172,25 @@
         <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="12">
+        <v>72</v>
+      </c>
+      <c r="C23" s="10">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="10">
         <f t="shared" si="2"/>
         <v>115</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="11">
         <f t="shared" si="3"/>
         <v>0.21000000000000005</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="11">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="11">
         <f t="shared" si="3"/>
         <v>0.21000000000000005</v>
       </c>
@@ -3196,7 +3198,7 @@
         <v>0.45500000000000002</v>
       </c>
       <c r="I23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3204,25 +3206,25 @@
         <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="12">
+        <v>74</v>
+      </c>
+      <c r="C24" s="10">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="10">
         <f t="shared" si="2"/>
         <v>120</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="11">
         <f t="shared" si="3"/>
         <v>0.22000000000000006</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="11">
         <f t="shared" si="0"/>
         <v>0.03</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="11">
         <f t="shared" si="3"/>
         <v>0.22000000000000006</v>
       </c>
@@ -3230,7 +3232,7 @@
         <v>0.71299999999999997</v>
       </c>
       <c r="I24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3238,25 +3240,25 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="12">
+        <v>73</v>
+      </c>
+      <c r="C25" s="10">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="10">
         <f t="shared" si="2"/>
         <v>125</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="11">
         <f t="shared" si="3"/>
         <v>0.23000000000000007</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="11">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
-      <c r="G25" s="13">
+      <c r="G25" s="11">
         <f t="shared" si="3"/>
         <v>0.23000000000000007</v>
       </c>
@@ -3264,7 +3266,7 @@
         <v>0.92900000000000005</v>
       </c>
       <c r="I25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3272,25 +3274,25 @@
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="12">
+        <v>73</v>
+      </c>
+      <c r="C26" s="10">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="10">
         <f t="shared" si="2"/>
         <v>130</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="11">
         <f t="shared" si="3"/>
         <v>0.24000000000000007</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="11">
         <f>F27+0.01</f>
         <v>0.01</v>
       </c>
-      <c r="G26" s="13">
+      <c r="G26" s="11">
         <f t="shared" si="3"/>
         <v>0.24000000000000007</v>
       </c>
@@ -3298,51 +3300,51 @@
         <v>0.89610000000000001</v>
       </c>
       <c r="I26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C31" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="10" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="12" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes + including GBR requests
</commit_message>
<xml_diff>
--- a/cfg/CPC_CONFIGURATIONS.xlsx
+++ b/cfg/CPC_CONFIGURATIONS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\IOTC working parties\iotc-tcac-simulations\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8F28CE-8BCB-4593-A1F3-93975894459D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35487B64-6042-4FAA-846B-06C301BB4AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1140" windowWidth="29040" windowHeight="15720" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
   </bookViews>
   <sheets>
     <sheet name="CPC" sheetId="1" r:id="rId1"/>
@@ -803,6 +803,7 @@
     <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.28515625" customWidth="1"/>
+    <col min="10" max="22" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -2412,9 +2413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6A7977-2381-4943-AA16-A4F852F13E83}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2429,31 +2428,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="6" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3355,6 +3354,7 @@
     <hyperlink ref="C31" r:id="rId4" xr:uid="{4A9C1AAE-88CB-4671-8792-DBBE075D16B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <ignoredErrors>
     <ignoredError sqref="F3:F26" formula="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Correction of MDV status of SID
</commit_message>
<xml_diff>
--- a/cfg/CPC_CONFIGURATIONS.xlsx
+++ b/cfg/CPC_CONFIGURATIONS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\IOTC working parties\iotc-tcac-simulations\cfg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-tcac-simulations\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35487B64-6042-4FAA-846B-06C301BB4AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D2F421-EB21-44CF-9AEF-DBB7D030052A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
   </bookViews>
   <sheets>
     <sheet name="CPC" sheetId="1" r:id="rId1"/>
@@ -788,9 +788,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDC28B42-0D9A-4986-9B76-3F979445C853}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -848,7 +851,7 @@
       <c r="V1" s="12"/>
       <c r="W1" s="12"/>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -893,7 +896,7 @@
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -936,7 +939,7 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1022,7 +1025,7 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1065,7 +1068,7 @@
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1108,7 +1111,7 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1151,7 +1154,7 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1194,7 +1197,7 @@
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1237,7 +1240,7 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1280,7 +1283,7 @@
       <c r="Y11" s="5"/>
       <c r="Z11" s="5"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1323,7 +1326,7 @@
       <c r="Y12" s="5"/>
       <c r="Z12" s="5"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1366,7 +1369,7 @@
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1409,7 +1412,7 @@
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1452,7 +1455,7 @@
       <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1495,7 +1498,7 @@
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>63</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1581,7 +1584,7 @@
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1667,7 +1670,7 @@
       <c r="Y20" s="5"/>
       <c r="Z20" s="5"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1710,7 +1713,7 @@
       <c r="Y21" s="5"/>
       <c r="Z21" s="5"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1753,7 +1756,7 @@
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1796,7 +1799,7 @@
       <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1839,7 +1842,7 @@
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -1882,7 +1885,7 @@
       <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1968,7 +1971,7 @@
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -2011,7 +2014,7 @@
       <c r="Y28" s="5"/>
       <c r="Z28" s="5"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -2054,7 +2057,7 @@
       <c r="Y29" s="5"/>
       <c r="Z29" s="5"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -2097,7 +2100,7 @@
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -2400,6 +2403,13 @@
       <c r="V48" s="13"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H31" xr:uid="{DDC28B42-0D9A-4986-9B76-3F979445C853}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="J1:W1"/>
     <mergeCell ref="J2:V48"/>

</xml_diff>

<commit_message>
Changed CPC to CP for STATUS and added TWN
</commit_message>
<xml_diff>
--- a/cfg/CPC_CONFIGURATIONS.xlsx
+++ b/cfg/CPC_CONFIGURATIONS.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-tcac-simulations\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D2F421-EB21-44CF-9AEF-DBB7D030052A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EBD9FA-9A43-4D30-A121-DDA58C55407C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
   </bookViews>
   <sheets>
     <sheet name="CPC" sheetId="1" r:id="rId1"/>
     <sheet name="COASTAL_STATE_SOCIO_ECONOMIC" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CPC!$A$1:$H$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CPC!$A$1:$H$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="101">
   <si>
     <t>SIDS</t>
   </si>
@@ -231,9 +231,6 @@
     <t>South Africa</t>
   </si>
   <si>
-    <t>CPC</t>
-  </si>
-  <si>
     <t>CNCP</t>
   </si>
   <si>
@@ -325,6 +322,24 @@
   </si>
   <si>
     <t>HAS_NJA_IO</t>
+  </si>
+  <si>
+    <t>NJA_SIZE</t>
+  </si>
+  <si>
+    <t>NJA_IOTC_RELATIVE_SIZE</t>
+  </si>
+  <si>
+    <t>TWN</t>
+  </si>
+  <si>
+    <t>Taiwan,China</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>OBS</t>
   </si>
   <si>
     <t>USE [IOTC_master]
@@ -335,7 +350,7 @@
 SELECT 
     C.CODE, 
     C.NAME_EN,
-    CASE WHEN H.CONTRACTING_PARTY = 1 THEN 'CPC' ELSE 'CNCP' END AS [STATUS],
+    CASE WHEN H.CONTRACTING_PARTY = 1 THEN 'CP' ELSE 'CNCP' END AS [STATUS],
     CASE WHEN C.CODE = 'EUR' THEN 0 ELSE C.IS_COASTAL END AS COASTAL, 
     C.IS_COASTAL AS HAS_NJA_IO,
     C.IS_SIDS AS SIDS,
@@ -365,14 +380,10 @@
     A.CODE = CASE WHEN C.CODE = 'FRAT' THEN 'AUNJ_ATF' ELSE CONCAT('AUNJ_', C.CODE) END
 WHERE 
     H.WITHDRAWAL_DATE IS NULL
+-- Add TWN
+UNION SELECT 'TWN' AS CODE, 'Taiwan,China' AS NAME_EN, 'OBS' AS STATUS, 0 AS COASTAL, 0 AS HAS_NJA_IO, 0 AS SIDS, 0 AS NJA_SIZE, 0 AS NJA_IOTC_RELATIVE_SIZE
 ORDER BY 
     1 ASC</t>
-  </si>
-  <si>
-    <t>NJA_SIZE</t>
-  </si>
-  <si>
-    <t>NJA_IOTC_RELATIVE_SIZE</t>
   </si>
 </sst>
 </file>
@@ -788,28 +799,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDC28B42-0D9A-4986-9B76-3F979445C853}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:Z48"/>
+  <dimension ref="A1:Z49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2:V49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.28515625" customWidth="1"/>
-    <col min="10" max="22" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.33203125" customWidth="1"/>
+    <col min="10" max="21" width="0" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="33.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -817,25 +829,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="F1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>96</v>
-      </c>
       <c r="H1" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
@@ -851,7 +863,7 @@
       <c r="V1" s="12"/>
       <c r="W1" s="12"/>
     </row>
-    <row r="2" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -859,7 +871,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -877,7 +889,7 @@
         <v>7.6899999999999996E-2</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
@@ -896,7 +908,7 @@
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
     </row>
-    <row r="3" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -904,7 +916,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -939,7 +951,7 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -947,7 +959,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -982,7 +994,7 @@
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -990,7 +1002,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1025,7 +1037,7 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
     </row>
-    <row r="6" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1033,7 +1045,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1068,7 +1080,7 @@
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
     </row>
-    <row r="7" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1076,7 +1088,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1111,7 +1123,7 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1119,7 +1131,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1154,7 +1166,7 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row r="9" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1162,7 +1174,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1197,7 +1209,7 @@
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
     </row>
-    <row r="10" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1205,7 +1217,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1240,7 +1252,7 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
     </row>
-    <row r="11" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1248,7 +1260,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1283,7 +1295,7 @@
       <c r="Y11" s="5"/>
       <c r="Z11" s="5"/>
     </row>
-    <row r="12" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1291,7 +1303,7 @@
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1326,7 +1338,7 @@
       <c r="Y12" s="5"/>
       <c r="Z12" s="5"/>
     </row>
-    <row r="13" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1334,7 +1346,7 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1369,7 +1381,7 @@
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
     </row>
-    <row r="14" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1377,7 +1389,7 @@
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1412,7 +1424,7 @@
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
     </row>
-    <row r="15" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1420,7 +1432,7 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1455,7 +1467,7 @@
       <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
     </row>
-    <row r="16" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1463,7 +1475,7 @@
         <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1498,7 +1510,7 @@
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
     </row>
-    <row r="17" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1506,7 +1518,7 @@
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1541,7 +1553,7 @@
       <c r="Y17" s="5"/>
       <c r="Z17" s="5"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1549,7 +1561,7 @@
         <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1584,7 +1596,7 @@
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
     </row>
-    <row r="19" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1592,7 +1604,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1627,7 +1639,7 @@
       <c r="Y19" s="5"/>
       <c r="Z19" s="5"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1635,7 +1647,7 @@
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1670,7 +1682,7 @@
       <c r="Y20" s="5"/>
       <c r="Z20" s="5"/>
     </row>
-    <row r="21" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1678,7 +1690,7 @@
         <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1713,7 +1725,7 @@
       <c r="Y21" s="5"/>
       <c r="Z21" s="5"/>
     </row>
-    <row r="22" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1721,7 +1733,7 @@
         <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1756,7 +1768,7 @@
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
     </row>
-    <row r="23" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1764,7 +1776,7 @@
         <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1799,7 +1811,7 @@
       <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
     </row>
-    <row r="24" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1807,7 +1819,7 @@
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1842,7 +1854,7 @@
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
     </row>
-    <row r="25" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -1850,7 +1862,7 @@
         <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1885,7 +1897,7 @@
       <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
     </row>
-    <row r="26" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1893,7 +1905,7 @@
         <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1928,7 +1940,7 @@
       <c r="Y26" s="5"/>
       <c r="Z26" s="5"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -1936,7 +1948,7 @@
         <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1971,7 +1983,7 @@
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
     </row>
-    <row r="28" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -1979,7 +1991,7 @@
         <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2014,30 +2026,30 @@
       <c r="Y28" s="5"/>
       <c r="Z28" s="5"/>
     </row>
-    <row r="29" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29">
-        <v>240763</v>
+        <v>0</v>
       </c>
       <c r="H29" s="2">
-        <v>3.8999999999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
@@ -2057,15 +2069,15 @@
       <c r="Y29" s="5"/>
       <c r="Z29" s="5"/>
     </row>
-    <row r="30" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2077,10 +2089,10 @@
         <v>1</v>
       </c>
       <c r="G30">
-        <v>543647</v>
+        <v>240763</v>
       </c>
       <c r="H30" s="2">
-        <v>8.8000000000000005E-3</v>
+        <v>3.8999999999999998E-3</v>
       </c>
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
@@ -2100,15 +2112,15 @@
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
     </row>
-    <row r="31" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2120,10 +2132,10 @@
         <v>1</v>
       </c>
       <c r="G31">
-        <v>781573</v>
+        <v>543647</v>
       </c>
       <c r="H31" s="2">
-        <v>1.89E-2</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
@@ -2143,7 +2155,31 @@
       <c r="Y31" s="5"/>
       <c r="Z31" s="5"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>781573</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1.89E-2</v>
+      </c>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
@@ -2162,7 +2198,7 @@
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
     </row>
-    <row r="33" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
@@ -2176,8 +2212,12 @@
       <c r="T33" s="13"/>
       <c r="U33" s="13"/>
       <c r="V33" s="13"/>
-    </row>
-    <row r="34" spans="10:22" x14ac:dyDescent="0.25">
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
+    </row>
+    <row r="34" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
       <c r="L34" s="13"/>
@@ -2192,7 +2232,7 @@
       <c r="U34" s="13"/>
       <c r="V34" s="13"/>
     </row>
-    <row r="35" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
@@ -2207,7 +2247,7 @@
       <c r="U35" s="13"/>
       <c r="V35" s="13"/>
     </row>
-    <row r="36" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
@@ -2222,7 +2262,7 @@
       <c r="U36" s="13"/>
       <c r="V36" s="13"/>
     </row>
-    <row r="37" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J37" s="13"/>
       <c r="K37" s="13"/>
       <c r="L37" s="13"/>
@@ -2237,7 +2277,7 @@
       <c r="U37" s="13"/>
       <c r="V37" s="13"/>
     </row>
-    <row r="38" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J38" s="13"/>
       <c r="K38" s="13"/>
       <c r="L38" s="13"/>
@@ -2252,7 +2292,7 @@
       <c r="U38" s="13"/>
       <c r="V38" s="13"/>
     </row>
-    <row r="39" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J39" s="13"/>
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
@@ -2267,7 +2307,7 @@
       <c r="U39" s="13"/>
       <c r="V39" s="13"/>
     </row>
-    <row r="40" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J40" s="13"/>
       <c r="K40" s="13"/>
       <c r="L40" s="13"/>
@@ -2282,7 +2322,7 @@
       <c r="U40" s="13"/>
       <c r="V40" s="13"/>
     </row>
-    <row r="41" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J41" s="13"/>
       <c r="K41" s="13"/>
       <c r="L41" s="13"/>
@@ -2297,7 +2337,7 @@
       <c r="U41" s="13"/>
       <c r="V41" s="13"/>
     </row>
-    <row r="42" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J42" s="13"/>
       <c r="K42" s="13"/>
       <c r="L42" s="13"/>
@@ -2312,7 +2352,7 @@
       <c r="U42" s="13"/>
       <c r="V42" s="13"/>
     </row>
-    <row r="43" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J43" s="13"/>
       <c r="K43" s="13"/>
       <c r="L43" s="13"/>
@@ -2327,7 +2367,7 @@
       <c r="U43" s="13"/>
       <c r="V43" s="13"/>
     </row>
-    <row r="44" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J44" s="13"/>
       <c r="K44" s="13"/>
       <c r="L44" s="13"/>
@@ -2342,7 +2382,7 @@
       <c r="U44" s="13"/>
       <c r="V44" s="13"/>
     </row>
-    <row r="45" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J45" s="13"/>
       <c r="K45" s="13"/>
       <c r="L45" s="13"/>
@@ -2357,7 +2397,7 @@
       <c r="U45" s="13"/>
       <c r="V45" s="13"/>
     </row>
-    <row r="46" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J46" s="13"/>
       <c r="K46" s="13"/>
       <c r="L46" s="13"/>
@@ -2372,7 +2412,7 @@
       <c r="U46" s="13"/>
       <c r="V46" s="13"/>
     </row>
-    <row r="47" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J47" s="13"/>
       <c r="K47" s="13"/>
       <c r="L47" s="13"/>
@@ -2387,7 +2427,7 @@
       <c r="U47" s="13"/>
       <c r="V47" s="13"/>
     </row>
-    <row r="48" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J48" s="13"/>
       <c r="K48" s="13"/>
       <c r="L48" s="13"/>
@@ -2402,17 +2442,25 @@
       <c r="U48" s="13"/>
       <c r="V48" s="13"/>
     </row>
+    <row r="49" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="13"/>
+      <c r="P49" s="13"/>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="13"/>
+      <c r="S49" s="13"/>
+      <c r="T49" s="13"/>
+      <c r="U49" s="13"/>
+      <c r="V49" s="13"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H31" xr:uid="{DDC28B42-0D9A-4986-9B76-3F979445C853}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="J1:W1"/>
-    <mergeCell ref="J2:V48"/>
+    <mergeCell ref="J2:V49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2421,57 +2469,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6A7977-2381-4943-AA16-A4F852F13E83}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
     <col min="5" max="5" width="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="10">
         <v>1</v>
@@ -2493,15 +2543,15 @@
         <v>0.95099999999999996</v>
       </c>
       <c r="I2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="10">
         <f>C2+1</f>
@@ -2527,15 +2577,15 @@
         <v>0.66100000000000003</v>
       </c>
       <c r="I3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="10">
         <f t="shared" ref="C4:C26" si="1">C3+1</f>
@@ -2561,15 +2611,15 @@
         <v>0.55800000000000005</v>
       </c>
       <c r="I4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="10">
         <f t="shared" si="1"/>
@@ -2595,15 +2645,15 @@
         <v>0.90300000000000002</v>
       </c>
       <c r="I5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="10">
         <f t="shared" si="1"/>
@@ -2629,15 +2679,15 @@
         <v>0.70499999999999996</v>
       </c>
       <c r="I6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="10">
         <f t="shared" si="1"/>
@@ -2663,15 +2713,15 @@
         <v>0.63300000000000001</v>
       </c>
       <c r="I7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="10">
         <f t="shared" si="1"/>
@@ -2697,15 +2747,15 @@
         <v>0.77400000000000002</v>
       </c>
       <c r="I8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="10">
         <f t="shared" si="1"/>
@@ -2731,15 +2781,15 @@
         <v>0.57499999999999996</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="10">
         <f t="shared" si="1"/>
@@ -2765,15 +2815,15 @@
         <v>0.78200000000000003</v>
       </c>
       <c r="I10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="10">
         <f t="shared" si="1"/>
@@ -2799,15 +2849,15 @@
         <v>0.501</v>
       </c>
       <c r="I11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="10">
         <f t="shared" si="1"/>
@@ -2833,15 +2883,15 @@
         <v>0.747</v>
       </c>
       <c r="I12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="10">
         <f t="shared" si="1"/>
@@ -2867,15 +2917,15 @@
         <v>0.44600000000000001</v>
       </c>
       <c r="I13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="10">
         <f t="shared" si="1"/>
@@ -2901,15 +2951,15 @@
         <v>0.80200000000000005</v>
       </c>
       <c r="I14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="10">
         <f t="shared" si="1"/>
@@ -2935,15 +2985,15 @@
         <v>0.80300000000000005</v>
       </c>
       <c r="I15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="10">
         <f t="shared" si="1"/>
@@ -2969,15 +3019,15 @@
         <v>0.81599999999999995</v>
       </c>
       <c r="I16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" s="10">
         <f t="shared" si="1"/>
@@ -3003,15 +3053,15 @@
         <v>0.54400000000000004</v>
       </c>
       <c r="I17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="10">
         <f t="shared" si="1"/>
@@ -3037,15 +3087,15 @@
         <v>0.50800000000000001</v>
       </c>
       <c r="I18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19" s="10">
         <f t="shared" si="1"/>
@@ -3068,18 +3118,18 @@
         <v>0.17</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="10">
         <f t="shared" si="1"/>
@@ -3105,15 +3155,15 @@
         <v>0.78500000000000003</v>
       </c>
       <c r="I20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="10">
         <f t="shared" si="1"/>
@@ -3139,15 +3189,15 @@
         <v>0.8</v>
       </c>
       <c r="I21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C22" s="10">
         <f t="shared" si="1"/>
@@ -3173,15 +3223,15 @@
         <v>0.54900000000000004</v>
       </c>
       <c r="I22" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C23" s="10">
         <f t="shared" si="1"/>
@@ -3207,15 +3257,15 @@
         <v>0.45500000000000002</v>
       </c>
       <c r="I23" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" s="10">
         <f t="shared" si="1"/>
@@ -3241,15 +3291,15 @@
         <v>0.71299999999999997</v>
       </c>
       <c r="I24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" s="10">
         <f t="shared" si="1"/>
@@ -3275,15 +3325,15 @@
         <v>0.92900000000000005</v>
       </c>
       <c r="I25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="10">
         <f t="shared" si="1"/>
@@ -3309,59 +3359,69 @@
         <v>0.89610000000000001</v>
       </c>
       <c r="I26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" t="s">
+        <v>72</v>
+      </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B28" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="8" t="s">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="C31" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="8" t="s">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="10" t="s">
-        <v>93</v>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="10" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C29" r:id="rId1" location="/indicies/HDI" xr:uid="{F6EE9713-CEE8-46D8-AB1C-C532ED013097}"/>
-    <hyperlink ref="C28" r:id="rId2" xr:uid="{BCADE41B-5E48-4B1E-80A6-096D888110A6}"/>
-    <hyperlink ref="C30" r:id="rId3" xr:uid="{732B9647-CC57-4B9A-8E3D-3752F3026E48}"/>
-    <hyperlink ref="C31" r:id="rId4" xr:uid="{4A9C1AAE-88CB-4671-8792-DBBE075D16B9}"/>
+    <hyperlink ref="C30" r:id="rId1" location="/indicies/HDI" xr:uid="{F6EE9713-CEE8-46D8-AB1C-C532ED013097}"/>
+    <hyperlink ref="C29" r:id="rId2" xr:uid="{BCADE41B-5E48-4B1E-80A6-096D888110A6}"/>
+    <hyperlink ref="C31" r:id="rId3" xr:uid="{732B9647-CC57-4B9A-8E3D-3752F3026E48}"/>
+    <hyperlink ref="C32" r:id="rId4" xr:uid="{4A9C1AAE-88CB-4671-8792-DBBE075D16B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
Inclusion of TWN in configuration files
</commit_message>
<xml_diff>
--- a/cfg/CPC_CONFIGURATIONS.xlsx
+++ b/cfg/CPC_CONFIGURATIONS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-tcac-simulations\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EBD9FA-9A43-4D30-A121-DDA58C55407C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3171DAD2-5401-46FB-9314-9C74B1331813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="341" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
   </bookViews>
   <sheets>
     <sheet name="CPC" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="101">
   <si>
     <t>SIDS</t>
   </si>
@@ -803,7 +803,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2:V49"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1051,7 +1051,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -2469,10 +2469,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6A7977-2381-4943-AA16-A4F852F13E83}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2533,7 +2533,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="11">
-        <f t="shared" ref="F2:F25" si="0">F3+0.01</f>
+        <f>F3+0.01</f>
         <v>0.25000000000000006</v>
       </c>
       <c r="G2" s="11">
@@ -2566,7 +2566,7 @@
         <v>0.01</v>
       </c>
       <c r="F3" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F3:F26" si="0">F4+0.01</f>
         <v>0.24000000000000007</v>
       </c>
       <c r="G3" s="11">
@@ -3348,7 +3348,7 @@
         <v>0.24000000000000007</v>
       </c>
       <c r="F26" s="11">
-        <f>F27+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="G26" s="11">
@@ -3363,70 +3363,57 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" t="s">
-        <v>72</v>
-      </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>74</v>
-      </c>
       <c r="B29" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" s="10" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="10" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C30" r:id="rId1" location="/indicies/HDI" xr:uid="{F6EE9713-CEE8-46D8-AB1C-C532ED013097}"/>
-    <hyperlink ref="C29" r:id="rId2" xr:uid="{BCADE41B-5E48-4B1E-80A6-096D888110A6}"/>
-    <hyperlink ref="C31" r:id="rId3" xr:uid="{732B9647-CC57-4B9A-8E3D-3752F3026E48}"/>
-    <hyperlink ref="C32" r:id="rId4" xr:uid="{4A9C1AAE-88CB-4671-8792-DBBE075D16B9}"/>
+    <hyperlink ref="C29" r:id="rId1" location="/indicies/HDI" xr:uid="{F6EE9713-CEE8-46D8-AB1C-C532ED013097}"/>
+    <hyperlink ref="C28" r:id="rId2" xr:uid="{BCADE41B-5E48-4B1E-80A6-096D888110A6}"/>
+    <hyperlink ref="C30" r:id="rId3" xr:uid="{732B9647-CC57-4B9A-8E3D-3752F3026E48}"/>
+    <hyperlink ref="C31" r:id="rId4" xr:uid="{4A9C1AAE-88CB-4671-8792-DBBE075D16B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-  <ignoredErrors>
-    <ignoredError sqref="F3:F26" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update of historical catch estimates to separate TWN from CHN
</commit_message>
<xml_diff>
--- a/cfg/CPC_CONFIGURATIONS.xlsx
+++ b/cfg/CPC_CONFIGURATIONS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-tcac-simulations\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3171DAD2-5401-46FB-9314-9C74B1331813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AA7AD4-316F-43E7-9888-69E0A6FCD27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="341" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
   </bookViews>
   <sheets>
     <sheet name="CPC" sheetId="1" r:id="rId1"/>
@@ -324,24 +324,6 @@
     <t>HAS_NJA_IO</t>
   </si>
   <si>
-    <t>NJA_SIZE</t>
-  </si>
-  <si>
-    <t>NJA_IOTC_RELATIVE_SIZE</t>
-  </si>
-  <si>
-    <t>TWN</t>
-  </si>
-  <si>
-    <t>Taiwan,China</t>
-  </si>
-  <si>
-    <t>CP</t>
-  </si>
-  <si>
-    <t>OBS</t>
-  </si>
-  <si>
     <t>USE [IOTC_master]
 DECLARE @IOTC_AREA FLOAT
 SET @IOTC_AREA = ( SELECT OCEAN_AREA_IOTC_KM2 FROM [IOTC_master].refs_gis.AREAS WHERE CODE LIKE 'IOTC_ALL' )
@@ -350,7 +332,7 @@
 SELECT 
     C.CODE, 
     C.NAME_EN,
-    CASE WHEN H.CONTRACTING_PARTY = 1 THEN 'CP' ELSE 'CNCP' END AS [STATUS],
+    CASE WHEN H.CONTRACTING_PARTY = 1 THEN 'CPC' ELSE 'CNCP' END AS [STATUS],
     CASE WHEN C.CODE = 'EUR' THEN 0 ELSE C.IS_COASTAL END AS COASTAL, 
     C.IS_COASTAL AS HAS_NJA_IO,
     C.IS_SIDS AS SIDS,
@@ -380,10 +362,26 @@
     A.CODE = CASE WHEN C.CODE = 'FRAT' THEN 'AUNJ_ATF' ELSE CONCAT('AUNJ_', C.CODE) END
 WHERE 
     H.WITHDRAWAL_DATE IS NULL
--- Add TWN
-UNION SELECT 'TWN' AS CODE, 'Taiwan,China' AS NAME_EN, 'OBS' AS STATUS, 0 AS COASTAL, 0 AS HAS_NJA_IO, 0 AS SIDS, 0 AS NJA_SIZE, 0 AS NJA_IOTC_RELATIVE_SIZE
 ORDER BY 
     1 ASC</t>
+  </si>
+  <si>
+    <t>NJA_SIZE</t>
+  </si>
+  <si>
+    <t>NJA_IOTC_RELATIVE_SIZE</t>
+  </si>
+  <si>
+    <t>TWN</t>
+  </si>
+  <si>
+    <t>Taiwan Province of China</t>
+  </si>
+  <si>
+    <t>OBS</t>
+  </si>
+  <si>
+    <t>CP</t>
   </si>
 </sst>
 </file>
@@ -802,26 +800,24 @@
   <dimension ref="A1:Z49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.33203125" customWidth="1"/>
-    <col min="10" max="21" width="0" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="33.44140625" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.28515625" customWidth="1"/>
+    <col min="10" max="22" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -841,10 +837,10 @@
         <v>93</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>82</v>
@@ -863,7 +859,7 @@
       <c r="V1" s="12"/>
       <c r="W1" s="12"/>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -871,7 +867,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -889,7 +885,7 @@
         <v>7.6899999999999996E-2</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
@@ -908,7 +904,7 @@
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -916,7 +912,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -951,7 +947,7 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -959,7 +955,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -994,7 +990,7 @@
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1002,7 +998,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1037,7 +1033,7 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1045,13 +1041,13 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1080,7 +1076,7 @@
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1088,7 +1084,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1123,7 +1119,7 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1131,7 +1127,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1166,7 +1162,7 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1174,7 +1170,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1209,7 +1205,7 @@
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1217,7 +1213,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1252,7 +1248,7 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1260,7 +1256,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1295,7 +1291,7 @@
       <c r="Y11" s="5"/>
       <c r="Z11" s="5"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1303,7 +1299,7 @@
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1338,7 +1334,7 @@
       <c r="Y12" s="5"/>
       <c r="Z12" s="5"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1346,7 +1342,7 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1381,7 +1377,7 @@
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1389,7 +1385,7 @@
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1424,7 +1420,7 @@
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1467,7 +1463,7 @@
       <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1475,7 +1471,7 @@
         <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1510,7 +1506,7 @@
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1518,7 +1514,7 @@
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1553,7 +1549,7 @@
       <c r="Y17" s="5"/>
       <c r="Z17" s="5"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1561,7 +1557,7 @@
         <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1596,7 +1592,7 @@
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1604,7 +1600,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1639,7 +1635,7 @@
       <c r="Y19" s="5"/>
       <c r="Z19" s="5"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1647,7 +1643,7 @@
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1682,7 +1678,7 @@
       <c r="Y20" s="5"/>
       <c r="Z20" s="5"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1690,7 +1686,7 @@
         <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1725,7 +1721,7 @@
       <c r="Y21" s="5"/>
       <c r="Z21" s="5"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1733,7 +1729,7 @@
         <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1768,7 +1764,7 @@
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1776,7 +1772,7 @@
         <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1811,7 +1807,7 @@
       <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1819,7 +1815,7 @@
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1854,7 +1850,7 @@
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -1862,7 +1858,7 @@
         <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1897,7 +1893,7 @@
       <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1905,7 +1901,7 @@
         <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1940,7 +1936,7 @@
       <c r="Y26" s="5"/>
       <c r="Z26" s="5"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -1948,7 +1944,7 @@
         <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1983,30 +1979,30 @@
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28">
-        <v>118137</v>
+        <v>0</v>
       </c>
       <c r="H28" s="2">
-        <v>1.9E-3</v>
+        <v>0</v>
       </c>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
@@ -2026,30 +2022,30 @@
       <c r="Y28" s="5"/>
       <c r="Z28" s="5"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>118137</v>
       </c>
       <c r="H29" s="2">
-        <v>0</v>
+        <v>1.9E-3</v>
       </c>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
@@ -2069,7 +2065,7 @@
       <c r="Y29" s="5"/>
       <c r="Z29" s="5"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -2077,7 +2073,7 @@
         <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2112,7 +2108,7 @@
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -2120,7 +2116,7 @@
         <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2155,7 +2151,7 @@
       <c r="Y31" s="5"/>
       <c r="Z31" s="5"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -2163,7 +2159,7 @@
         <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2198,7 +2194,7 @@
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
     </row>
-    <row r="33" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
@@ -2217,7 +2213,7 @@
       <c r="Y33" s="5"/>
       <c r="Z33" s="5"/>
     </row>
-    <row r="34" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
       <c r="L34" s="13"/>
@@ -2232,7 +2228,7 @@
       <c r="U34" s="13"/>
       <c r="V34" s="13"/>
     </row>
-    <row r="35" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
@@ -2247,7 +2243,7 @@
       <c r="U35" s="13"/>
       <c r="V35" s="13"/>
     </row>
-    <row r="36" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
@@ -2262,7 +2258,7 @@
       <c r="U36" s="13"/>
       <c r="V36" s="13"/>
     </row>
-    <row r="37" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J37" s="13"/>
       <c r="K37" s="13"/>
       <c r="L37" s="13"/>
@@ -2277,7 +2273,7 @@
       <c r="U37" s="13"/>
       <c r="V37" s="13"/>
     </row>
-    <row r="38" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J38" s="13"/>
       <c r="K38" s="13"/>
       <c r="L38" s="13"/>
@@ -2292,7 +2288,7 @@
       <c r="U38" s="13"/>
       <c r="V38" s="13"/>
     </row>
-    <row r="39" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J39" s="13"/>
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
@@ -2307,7 +2303,7 @@
       <c r="U39" s="13"/>
       <c r="V39" s="13"/>
     </row>
-    <row r="40" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J40" s="13"/>
       <c r="K40" s="13"/>
       <c r="L40" s="13"/>
@@ -2322,7 +2318,7 @@
       <c r="U40" s="13"/>
       <c r="V40" s="13"/>
     </row>
-    <row r="41" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J41" s="13"/>
       <c r="K41" s="13"/>
       <c r="L41" s="13"/>
@@ -2337,7 +2333,7 @@
       <c r="U41" s="13"/>
       <c r="V41" s="13"/>
     </row>
-    <row r="42" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J42" s="13"/>
       <c r="K42" s="13"/>
       <c r="L42" s="13"/>
@@ -2352,7 +2348,7 @@
       <c r="U42" s="13"/>
       <c r="V42" s="13"/>
     </row>
-    <row r="43" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J43" s="13"/>
       <c r="K43" s="13"/>
       <c r="L43" s="13"/>
@@ -2367,7 +2363,7 @@
       <c r="U43" s="13"/>
       <c r="V43" s="13"/>
     </row>
-    <row r="44" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J44" s="13"/>
       <c r="K44" s="13"/>
       <c r="L44" s="13"/>
@@ -2382,7 +2378,7 @@
       <c r="U44" s="13"/>
       <c r="V44" s="13"/>
     </row>
-    <row r="45" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J45" s="13"/>
       <c r="K45" s="13"/>
       <c r="L45" s="13"/>
@@ -2397,7 +2393,7 @@
       <c r="U45" s="13"/>
       <c r="V45" s="13"/>
     </row>
-    <row r="46" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J46" s="13"/>
       <c r="K46" s="13"/>
       <c r="L46" s="13"/>
@@ -2412,7 +2408,7 @@
       <c r="U46" s="13"/>
       <c r="V46" s="13"/>
     </row>
-    <row r="47" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J47" s="13"/>
       <c r="K47" s="13"/>
       <c r="L47" s="13"/>
@@ -2427,7 +2423,7 @@
       <c r="U47" s="13"/>
       <c r="V47" s="13"/>
     </row>
-    <row r="48" spans="10:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="10:26" x14ac:dyDescent="0.25">
       <c r="J48" s="13"/>
       <c r="K48" s="13"/>
       <c r="L48" s="13"/>
@@ -2442,7 +2438,7 @@
       <c r="U48" s="13"/>
       <c r="V48" s="13"/>
     </row>
-    <row r="49" spans="10:22" x14ac:dyDescent="0.3">
+    <row r="49" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J49" s="13"/>
       <c r="K49" s="13"/>
       <c r="L49" s="13"/>
@@ -2458,6 +2454,7 @@
       <c r="V49" s="13"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H32" xr:uid="{DDC28B42-0D9A-4986-9B76-3F979445C853}"/>
   <mergeCells count="2">
     <mergeCell ref="J1:W1"/>
     <mergeCell ref="J2:V49"/>
@@ -2471,23 +2468,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6A7977-2381-4943-AA16-A4F852F13E83}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2516,7 +2513,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2533,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="11">
-        <f>F3+0.01</f>
+        <f t="shared" ref="F2:F25" si="0">F3+0.01</f>
         <v>0.25000000000000006</v>
       </c>
       <c r="G2" s="11">
@@ -2546,7 +2543,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2566,7 +2563,7 @@
         <v>0.01</v>
       </c>
       <c r="F3" s="11">
-        <f t="shared" ref="F3:F26" si="0">F4+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.24000000000000007</v>
       </c>
       <c r="G3" s="11">
@@ -2580,7 +2577,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2614,7 +2611,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2648,7 +2645,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2682,7 +2679,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2716,7 +2713,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2750,7 +2747,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -2784,7 +2781,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2818,7 +2815,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -2852,7 +2849,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -2886,7 +2883,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -2920,7 +2917,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -2954,7 +2951,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -2988,7 +2985,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -3022,7 +3019,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -3056,7 +3053,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -3090,7 +3087,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -3124,7 +3121,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -3158,7 +3155,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -3192,7 +3189,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -3226,7 +3223,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -3260,7 +3257,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -3294,7 +3291,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -3328,7 +3325,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -3348,7 +3345,7 @@
         <v>0.24000000000000007</v>
       </c>
       <c r="F26" s="11">
-        <f t="shared" si="0"/>
+        <f>F27+0.01</f>
         <v>0.01</v>
       </c>
       <c r="G26" s="11">
@@ -3362,11 +3359,11 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -3377,7 +3374,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>77</v>
       </c>
@@ -3385,7 +3382,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>86</v>
       </c>
@@ -3393,7 +3390,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>83</v>
       </c>
@@ -3401,7 +3398,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
         <v>92</v>
       </c>
@@ -3415,5 +3412,8 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <ignoredErrors>
+    <ignoredError sqref="F3:F26" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update of EUR and GBR as "coastal" CPs
</commit_message>
<xml_diff>
--- a/cfg/CPC_CONFIGURATIONS.xlsx
+++ b/cfg/CPC_CONFIGURATIONS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-tcac-simulations\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AA7AD4-316F-43E7-9888-69E0A6FCD27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F9FBE6-DF70-4C84-8836-B2D5E4E70792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
   </bookViews>
   <sheets>
     <sheet name="CPC" sheetId="1" r:id="rId1"/>
@@ -800,7 +800,7 @@
   <dimension ref="A1:Z49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,7 +1047,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1133,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -2468,9 +2468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6A7977-2381-4943-AA16-A4F852F13E83}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Full revision of ReadMe file to be provided as document for the TCAC
</commit_message>
<xml_diff>
--- a/cfg/CPC_CONFIGURATIONS.xlsx
+++ b/cfg/CPC_CONFIGURATIONS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\iotc-tcac-simulations\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C65F06F-45EF-4E9F-A670-E533863C841C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B46FC86-1775-468A-A2CA-4FF29D29C11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
   </bookViews>
   <sheets>
     <sheet name="CPC" sheetId="1" r:id="rId1"/>
@@ -891,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDC28B42-0D9A-4986-9B76-3F979445C853}">
   <dimension ref="A1:AB49"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -900,10 +900,10 @@
     <col min="1" max="1" width="8.1796875" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.1796875" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.453125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.36328125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="7.1796875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.26953125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.26953125" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.26953125" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26" style="13" bestFit="1" customWidth="1"/>
@@ -2755,8 +2755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6A7977-2381-4943-AA16-A4F852F13E83}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2831,7 +2831,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="7">
-        <f>H3+0.01</f>
+        <f t="shared" ref="H2:H26" si="0">H3+0.01</f>
         <v>0.25000000000000006</v>
       </c>
       <c r="I2" s="7">
@@ -2858,23 +2858,23 @@
         <v>69</v>
       </c>
       <c r="E3" s="6">
-        <f>E2+1</f>
+        <f t="shared" ref="E3:E26" si="1">E2+1</f>
         <v>2</v>
       </c>
       <c r="F3" s="6">
-        <f>F2+5</f>
+        <f t="shared" ref="F3:F26" si="2">F2+5</f>
         <v>15</v>
       </c>
       <c r="G3" s="7">
-        <f>G2+0.01</f>
+        <f t="shared" ref="G3:G26" si="3">G2+0.01</f>
         <v>0.01</v>
       </c>
       <c r="H3" s="7">
-        <f>H4+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.24000000000000007</v>
       </c>
       <c r="I3" s="7">
-        <f>I2+0.01</f>
+        <f t="shared" ref="I3:I26" si="4">I2+0.01</f>
         <v>0.01</v>
       </c>
       <c r="J3" s="1">
@@ -2898,23 +2898,23 @@
         <v>69</v>
       </c>
       <c r="E4" s="6">
-        <f>E3+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="F4" s="6">
-        <f>F3+5</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="G4" s="7">
-        <f>G3+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
       <c r="H4" s="7">
-        <f>H5+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.23000000000000007</v>
       </c>
       <c r="I4" s="7">
-        <f>I3+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.02</v>
       </c>
       <c r="J4" s="1">
@@ -2938,23 +2938,23 @@
         <v>70</v>
       </c>
       <c r="E5" s="6">
-        <f>E4+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="F5" s="6">
-        <f>F4+5</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="G5" s="7">
-        <f>G4+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
       <c r="H5" s="7">
-        <f>H6+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.22000000000000006</v>
       </c>
       <c r="I5" s="7">
-        <f>I4+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.03</v>
       </c>
       <c r="J5" s="1">
@@ -2978,23 +2978,23 @@
         <v>70</v>
       </c>
       <c r="E6" s="6">
-        <f>E5+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="F6" s="6">
-        <f>F5+5</f>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="G6" s="7">
-        <f>G5+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
       <c r="H6" s="7">
-        <f>H7+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.21000000000000005</v>
       </c>
       <c r="I6" s="7">
-        <f>I5+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J6" s="1">
@@ -3018,23 +3018,23 @@
         <v>70</v>
       </c>
       <c r="E7" s="6">
-        <f>E6+1</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="F7" s="6">
-        <f>F6+5</f>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="G7" s="7">
-        <f>G6+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="H7" s="7">
-        <f>H8+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.20000000000000004</v>
       </c>
       <c r="I7" s="7">
-        <f>I6+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.05</v>
       </c>
       <c r="J7" s="1">
@@ -3058,23 +3058,23 @@
         <v>71</v>
       </c>
       <c r="E8" s="6">
-        <f>E7+1</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F8" s="6">
-        <f>F7+5</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="G8" s="7">
-        <f>G7+0.01</f>
+        <f t="shared" si="3"/>
         <v>6.0000000000000005E-2</v>
       </c>
       <c r="H8" s="7">
-        <f>H9+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.19000000000000003</v>
       </c>
       <c r="I8" s="7">
-        <f>I7+0.01</f>
+        <f t="shared" si="4"/>
         <v>6.0000000000000005E-2</v>
       </c>
       <c r="J8" s="1">
@@ -3098,23 +3098,23 @@
         <v>71</v>
       </c>
       <c r="E9" s="6">
-        <f>E8+1</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="F9" s="6">
-        <f>F8+5</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="G9" s="7">
-        <f>G8+0.01</f>
+        <f t="shared" si="3"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H9" s="7">
-        <f>H10+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.18000000000000002</v>
       </c>
       <c r="I9" s="7">
-        <f>I8+0.01</f>
+        <f t="shared" si="4"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="J9" s="1">
@@ -3138,23 +3138,23 @@
         <v>71</v>
       </c>
       <c r="E10" s="6">
-        <f>E9+1</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="F10" s="6">
-        <f>F9+5</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="G10" s="7">
-        <f>G9+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.08</v>
       </c>
       <c r="H10" s="7">
-        <f>H11+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
       <c r="I10" s="7">
-        <f>I9+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.08</v>
       </c>
       <c r="J10" s="1">
@@ -3178,23 +3178,23 @@
         <v>71</v>
       </c>
       <c r="E11" s="6">
-        <f>E10+1</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F11" s="6">
-        <f>F10+5</f>
+        <f t="shared" si="2"/>
         <v>55</v>
       </c>
       <c r="G11" s="7">
-        <f>G10+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.09</v>
       </c>
       <c r="H11" s="7">
-        <f>H12+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
       <c r="I11" s="7">
-        <f>I10+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.09</v>
       </c>
       <c r="J11" s="1">
@@ -3218,23 +3218,23 @@
         <v>71</v>
       </c>
       <c r="E12" s="6">
-        <f>E11+1</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="F12" s="6">
-        <f>F11+5</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="G12" s="7">
-        <f>G11+0.01</f>
+        <f t="shared" si="3"/>
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="H12" s="7">
-        <f>H13+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
       <c r="I12" s="7">
-        <f>I11+0.01</f>
+        <f t="shared" si="4"/>
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="J12" s="1">
@@ -3258,23 +3258,23 @@
         <v>69</v>
       </c>
       <c r="E13" s="6">
-        <f>E12+1</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="F13" s="6">
-        <f>F12+5</f>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="G13" s="7">
-        <f>G12+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.10999999999999999</v>
       </c>
       <c r="H13" s="7">
-        <f>H14+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.13999999999999999</v>
       </c>
       <c r="I13" s="7">
-        <f>I12+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.10999999999999999</v>
       </c>
       <c r="J13" s="1">
@@ -3298,23 +3298,23 @@
         <v>71</v>
       </c>
       <c r="E14" s="6">
-        <f>E13+1</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="F14" s="6">
-        <f>F13+5</f>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="G14" s="7">
-        <f>G13+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.11999999999999998</v>
       </c>
       <c r="H14" s="7">
-        <f>H15+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.12999999999999998</v>
       </c>
       <c r="I14" s="7">
-        <f>I13+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.11999999999999998</v>
       </c>
       <c r="J14" s="1">
@@ -3338,23 +3338,23 @@
         <v>69</v>
       </c>
       <c r="E15" s="6">
-        <f>E14+1</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="F15" s="6">
-        <f>F14+5</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="G15" s="7">
-        <f>G14+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.12999999999999998</v>
       </c>
       <c r="H15" s="7">
-        <f>H16+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.11999999999999998</v>
       </c>
       <c r="I15" s="7">
-        <f>I14+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.12999999999999998</v>
       </c>
       <c r="J15" s="1">
@@ -3378,23 +3378,23 @@
         <v>71</v>
       </c>
       <c r="E16" s="6">
-        <f>E15+1</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="F16" s="6">
-        <f>F15+5</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="G16" s="7">
-        <f>G15+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.13999999999999999</v>
       </c>
       <c r="H16" s="7">
-        <f>H17+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.10999999999999999</v>
       </c>
       <c r="I16" s="7">
-        <f>I15+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.13999999999999999</v>
       </c>
       <c r="J16" s="1">
@@ -3418,23 +3418,23 @@
         <v>71</v>
       </c>
       <c r="E17" s="6">
-        <f>E16+1</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="F17" s="6">
-        <f>F16+5</f>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="G17" s="7">
-        <f>G16+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
       <c r="H17" s="7">
-        <f>H18+0.01</f>
+        <f t="shared" si="0"/>
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="I17" s="7">
-        <f>I16+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.15</v>
       </c>
       <c r="J17" s="1">
@@ -3458,23 +3458,23 @@
         <v>71</v>
       </c>
       <c r="E18" s="6">
-        <f>E17+1</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="F18" s="6">
-        <f>F17+5</f>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="G18" s="7">
-        <f>G17+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.16</v>
       </c>
       <c r="H18" s="7">
-        <f>H19+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
       <c r="I18" s="7">
-        <f>I17+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.16</v>
       </c>
       <c r="J18" s="1">
@@ -3498,23 +3498,23 @@
         <v>71</v>
       </c>
       <c r="E19" s="6">
-        <f>E18+1</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="F19" s="6">
-        <f>F18+5</f>
+        <f t="shared" si="2"/>
         <v>95</v>
       </c>
       <c r="G19" s="7">
-        <f>G18+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.17</v>
       </c>
       <c r="H19" s="7">
-        <f>H20+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
       <c r="I19" s="7">
-        <f>I18+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.17</v>
       </c>
       <c r="J19" s="1">
@@ -3538,23 +3538,23 @@
         <v>69</v>
       </c>
       <c r="E20" s="6">
-        <f>E19+1</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="F20" s="6">
-        <f>F19+5</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G20" s="7">
-        <f>G19+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.18000000000000002</v>
       </c>
       <c r="H20" s="7">
-        <f>H21+0.01</f>
+        <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="I20" s="7">
-        <f>I19+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.18000000000000002</v>
       </c>
       <c r="J20" s="1">
@@ -3578,23 +3578,23 @@
         <v>69</v>
       </c>
       <c r="E21" s="6">
-        <f>E20+1</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F21" s="6">
-        <f>F20+5</f>
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="G21" s="7">
-        <f>G20+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.19000000000000003</v>
       </c>
       <c r="H21" s="7">
-        <f>H22+0.01</f>
+        <f t="shared" si="0"/>
         <v>6.0000000000000005E-2</v>
       </c>
       <c r="I21" s="7">
-        <f>I20+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.19000000000000003</v>
       </c>
       <c r="J21" s="2" t="s">
@@ -3618,23 +3618,23 @@
         <v>71</v>
       </c>
       <c r="E22" s="6">
-        <f>E21+1</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="F22" s="6">
-        <f>F21+5</f>
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
       <c r="G22" s="7">
-        <f>G21+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.20000000000000004</v>
       </c>
       <c r="H22" s="7">
-        <f>H23+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
       <c r="I22" s="7">
-        <f>I21+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.20000000000000004</v>
       </c>
       <c r="J22" s="1">
@@ -3658,23 +3658,23 @@
         <v>71</v>
       </c>
       <c r="E23" s="6">
-        <f>E22+1</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="F23" s="6">
-        <f>F22+5</f>
+        <f t="shared" si="2"/>
         <v>115</v>
       </c>
       <c r="G23" s="7">
-        <f>G22+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.21000000000000005</v>
       </c>
       <c r="H23" s="7">
-        <f>H24+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
       <c r="I23" s="7">
-        <f>I22+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.21000000000000005</v>
       </c>
       <c r="J23" s="1">
@@ -3698,23 +3698,23 @@
         <v>69</v>
       </c>
       <c r="E24" s="6">
-        <f>E23+1</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="F24" s="6">
-        <f>F23+5</f>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="G24" s="7">
-        <f>G23+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.22000000000000006</v>
       </c>
       <c r="H24" s="7">
-        <f>H25+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.03</v>
       </c>
       <c r="I24" s="7">
-        <f>I23+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.22000000000000006</v>
       </c>
       <c r="J24" s="1">
@@ -3738,23 +3738,23 @@
         <v>69</v>
       </c>
       <c r="E25" s="6">
-        <f>E24+1</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="F25" s="6">
-        <f>F24+5</f>
+        <f t="shared" si="2"/>
         <v>125</v>
       </c>
       <c r="G25" s="7">
-        <f>G24+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.23000000000000007</v>
       </c>
       <c r="H25" s="7">
-        <f>H26+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
       <c r="I25" s="7">
-        <f>I24+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.23000000000000007</v>
       </c>
       <c r="J25" s="1">
@@ -3778,23 +3778,23 @@
         <v>71</v>
       </c>
       <c r="E26" s="6">
-        <f>E25+1</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="F26" s="6">
-        <f>F25+5</f>
+        <f t="shared" si="2"/>
         <v>130</v>
       </c>
       <c r="G26" s="7">
-        <f>G25+0.01</f>
+        <f t="shared" si="3"/>
         <v>0.24000000000000007</v>
       </c>
       <c r="H26" s="7">
-        <f>H27+0.01</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="I26" s="7">
-        <f>I25+0.01</f>
+        <f t="shared" si="4"/>
         <v>0.24000000000000007</v>
       </c>
       <c r="J26" s="1">
@@ -3818,6 +3818,7 @@
       <c r="C28" s="4" t="s">
         <v>83</v>
       </c>
+      <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B29" t="s">

</xml_diff>

<commit_message>
Progress on simulation tool paper
</commit_message>
<xml_diff>
--- a/cfg/CPC_CONFIGURATIONS.xlsx
+++ b/cfg/CPC_CONFIGURATIONS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\iotc-tcac-simulations\cfg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\data-analysis\iotc-tcac-simulations\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B46FC86-1775-468A-A2CA-4FF29D29C11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D71BC8-713E-4F07-A9A8-327E9ABF5440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
   </bookViews>
   <sheets>
     <sheet name="CPC" sheetId="1" r:id="rId1"/>
@@ -891,28 +891,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDC28B42-0D9A-4986-9B76-3F979445C853}">
   <dimension ref="A1:AB49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.1796875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.453125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.7265625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.08984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.26953125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.26953125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.26953125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="3.28515625" style="10" customWidth="1"/>
     <col min="12" max="24" width="0" style="10" hidden="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.7265625" style="10"/>
+    <col min="25" max="16384" width="8.7109375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -960,7 +960,7 @@
       <c r="X1" s="14"/>
       <c r="Y1" s="14"/>
     </row>
-    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
@@ -1011,7 +1011,7 @@
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
@@ -1060,7 +1060,7 @@
       <c r="AA3" s="12"/>
       <c r="AB3" s="12"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
@@ -1109,7 +1109,7 @@
       <c r="AA4" s="12"/>
       <c r="AB4" s="12"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
@@ -1158,7 +1158,7 @@
       <c r="AA5" s="12"/>
       <c r="AB5" s="12"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
@@ -1207,7 +1207,7 @@
       <c r="AA6" s="12"/>
       <c r="AB6" s="12"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
@@ -1256,7 +1256,7 @@
       <c r="AA7" s="12"/>
       <c r="AB7" s="12"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
@@ -1305,7 +1305,7 @@
       <c r="AA8" s="12"/>
       <c r="AB8" s="12"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>16</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="AA9" s="12"/>
       <c r="AB9" s="12"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>18</v>
       </c>
@@ -1403,7 +1403,7 @@
       <c r="AA10" s="12"/>
       <c r="AB10" s="12"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
@@ -1452,7 +1452,7 @@
       <c r="AA11" s="12"/>
       <c r="AB11" s="12"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
@@ -1501,7 +1501,7 @@
       <c r="AA12" s="12"/>
       <c r="AB12" s="12"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>24</v>
       </c>
@@ -1550,7 +1550,7 @@
       <c r="AA13" s="12"/>
       <c r="AB13" s="12"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>26</v>
       </c>
@@ -1599,7 +1599,7 @@
       <c r="AA14" s="12"/>
       <c r="AB14" s="12"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>28</v>
       </c>
@@ -1648,7 +1648,7 @@
       <c r="AA15" s="12"/>
       <c r="AB15" s="12"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>30</v>
       </c>
@@ -1697,7 +1697,7 @@
       <c r="AA16" s="12"/>
       <c r="AB16" s="12"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>32</v>
       </c>
@@ -1746,7 +1746,7 @@
       <c r="AA17" s="12"/>
       <c r="AB17" s="12"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>34</v>
       </c>
@@ -1795,7 +1795,7 @@
       <c r="AA18" s="12"/>
       <c r="AB18" s="12"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>36</v>
       </c>
@@ -1844,7 +1844,7 @@
       <c r="AA19" s="12"/>
       <c r="AB19" s="12"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>38</v>
       </c>
@@ -1893,7 +1893,7 @@
       <c r="AA20" s="12"/>
       <c r="AB20" s="12"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>40</v>
       </c>
@@ -1942,7 +1942,7 @@
       <c r="AA21" s="12"/>
       <c r="AB21" s="12"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>42</v>
       </c>
@@ -1991,7 +1991,7 @@
       <c r="AA22" s="12"/>
       <c r="AB22" s="12"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>44</v>
       </c>
@@ -2040,7 +2040,7 @@
       <c r="AA23" s="12"/>
       <c r="AB23" s="12"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>46</v>
       </c>
@@ -2089,7 +2089,7 @@
       <c r="AA24" s="12"/>
       <c r="AB24" s="12"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>48</v>
       </c>
@@ -2138,7 +2138,7 @@
       <c r="AA25" s="12"/>
       <c r="AB25" s="12"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>50</v>
       </c>
@@ -2187,7 +2187,7 @@
       <c r="AA26" s="12"/>
       <c r="AB26" s="12"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>52</v>
       </c>
@@ -2236,7 +2236,7 @@
       <c r="AA27" s="12"/>
       <c r="AB27" s="12"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>95</v>
       </c>
@@ -2285,7 +2285,7 @@
       <c r="AA28" s="12"/>
       <c r="AB28" s="12"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>54</v>
       </c>
@@ -2334,7 +2334,7 @@
       <c r="AA29" s="12"/>
       <c r="AB29" s="12"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>56</v>
       </c>
@@ -2383,7 +2383,7 @@
       <c r="AA30" s="12"/>
       <c r="AB30" s="12"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>58</v>
       </c>
@@ -2432,7 +2432,7 @@
       <c r="AA31" s="12"/>
       <c r="AB31" s="12"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>60</v>
       </c>
@@ -2481,7 +2481,7 @@
       <c r="AA32" s="12"/>
       <c r="AB32" s="12"/>
     </row>
-    <row r="33" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="33" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L33" s="15"/>
       <c r="M33" s="15"/>
       <c r="N33" s="15"/>
@@ -2500,7 +2500,7 @@
       <c r="AA33" s="12"/>
       <c r="AB33" s="12"/>
     </row>
-    <row r="34" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="34" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
       <c r="N34" s="15"/>
@@ -2515,7 +2515,7 @@
       <c r="W34" s="15"/>
       <c r="X34" s="15"/>
     </row>
-    <row r="35" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="35" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
@@ -2530,7 +2530,7 @@
       <c r="W35" s="15"/>
       <c r="X35" s="15"/>
     </row>
-    <row r="36" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="36" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L36" s="15"/>
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
@@ -2545,7 +2545,7 @@
       <c r="W36" s="15"/>
       <c r="X36" s="15"/>
     </row>
-    <row r="37" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="37" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L37" s="15"/>
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
@@ -2560,7 +2560,7 @@
       <c r="W37" s="15"/>
       <c r="X37" s="15"/>
     </row>
-    <row r="38" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="38" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
       <c r="N38" s="15"/>
@@ -2575,7 +2575,7 @@
       <c r="W38" s="15"/>
       <c r="X38" s="15"/>
     </row>
-    <row r="39" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="39" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
@@ -2590,7 +2590,7 @@
       <c r="W39" s="15"/>
       <c r="X39" s="15"/>
     </row>
-    <row r="40" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="40" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
@@ -2605,7 +2605,7 @@
       <c r="W40" s="15"/>
       <c r="X40" s="15"/>
     </row>
-    <row r="41" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="41" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
       <c r="N41" s="15"/>
@@ -2620,7 +2620,7 @@
       <c r="W41" s="15"/>
       <c r="X41" s="15"/>
     </row>
-    <row r="42" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="42" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
       <c r="N42" s="15"/>
@@ -2635,7 +2635,7 @@
       <c r="W42" s="15"/>
       <c r="X42" s="15"/>
     </row>
-    <row r="43" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="43" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
       <c r="N43" s="15"/>
@@ -2650,7 +2650,7 @@
       <c r="W43" s="15"/>
       <c r="X43" s="15"/>
     </row>
-    <row r="44" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="44" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L44" s="15"/>
       <c r="M44" s="15"/>
       <c r="N44" s="15"/>
@@ -2665,7 +2665,7 @@
       <c r="W44" s="15"/>
       <c r="X44" s="15"/>
     </row>
-    <row r="45" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="45" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L45" s="15"/>
       <c r="M45" s="15"/>
       <c r="N45" s="15"/>
@@ -2680,7 +2680,7 @@
       <c r="W45" s="15"/>
       <c r="X45" s="15"/>
     </row>
-    <row r="46" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="46" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
       <c r="N46" s="15"/>
@@ -2695,7 +2695,7 @@
       <c r="W46" s="15"/>
       <c r="X46" s="15"/>
     </row>
-    <row r="47" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="47" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
       <c r="N47" s="15"/>
@@ -2710,7 +2710,7 @@
       <c r="W47" s="15"/>
       <c r="X47" s="15"/>
     </row>
-    <row r="48" spans="12:28" x14ac:dyDescent="0.35">
+    <row r="48" spans="12:28" x14ac:dyDescent="0.25">
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
       <c r="N48" s="15"/>
@@ -2725,7 +2725,7 @@
       <c r="W48" s="15"/>
       <c r="X48" s="15"/>
     </row>
-    <row r="49" spans="12:24" x14ac:dyDescent="0.35">
+    <row r="49" spans="12:24" x14ac:dyDescent="0.25">
       <c r="L49" s="15"/>
       <c r="M49" s="15"/>
       <c r="N49" s="15"/>
@@ -2755,25 +2755,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6A7977-2381-4943-AA16-A4F852F13E83}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.1796875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.1796875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="46.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" style="10" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.26953125" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2824,9 +2824,7 @@
       <c r="E2" s="6">
         <v>1</v>
       </c>
-      <c r="F2" s="6">
-        <v>10</v>
-      </c>
+      <c r="F2" s="10"/>
       <c r="G2" s="7">
         <v>0</v>
       </c>
@@ -2844,7 +2842,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2861,12 +2859,11 @@
         <f t="shared" ref="E3:E26" si="1">E2+1</f>
         <v>2</v>
       </c>
-      <c r="F3" s="6">
-        <f t="shared" ref="F3:F26" si="2">F2+5</f>
-        <v>15</v>
+      <c r="F3" s="10">
+        <v>0.94</v>
       </c>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G26" si="3">G2+0.01</f>
+        <f t="shared" ref="G3:G26" si="2">G2+0.01</f>
         <v>0.01</v>
       </c>
       <c r="H3" s="7">
@@ -2874,7 +2871,7 @@
         <v>0.24000000000000007</v>
       </c>
       <c r="I3" s="7">
-        <f t="shared" ref="I3:I26" si="4">I2+0.01</f>
+        <f t="shared" ref="I3:I26" si="3">I2+0.01</f>
         <v>0.01</v>
       </c>
       <c r="J3" s="1">
@@ -2884,7 +2881,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2901,12 +2898,11 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="10">
+        <v>0.77</v>
+      </c>
+      <c r="G4" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
       <c r="H4" s="7">
@@ -2914,7 +2910,7 @@
         <v>0.23000000000000007</v>
       </c>
       <c r="I4" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
       <c r="J4" s="1">
@@ -2924,7 +2920,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2941,12 +2937,9 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="10"/>
+      <c r="G5" s="7">
         <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="G5" s="7">
-        <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
       <c r="H5" s="7">
@@ -2954,7 +2947,7 @@
         <v>0.22000000000000006</v>
       </c>
       <c r="I5" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
       <c r="J5" s="1">
@@ -2964,7 +2957,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2981,12 +2974,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="10"/>
+      <c r="G6" s="7">
         <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="G6" s="7">
-        <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
       <c r="H6" s="7">
@@ -2994,7 +2984,7 @@
         <v>0.21000000000000005</v>
       </c>
       <c r="I6" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
       <c r="J6" s="1">
@@ -3004,7 +2994,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -3021,12 +3011,9 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="10"/>
+      <c r="G7" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-      <c r="G7" s="7">
-        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="H7" s="7">
@@ -3034,7 +3021,7 @@
         <v>0.20000000000000004</v>
       </c>
       <c r="I7" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="J7" s="1">
@@ -3044,7 +3031,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -3061,12 +3048,11 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="10">
+        <v>0.47</v>
+      </c>
+      <c r="G8" s="7">
         <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="G8" s="7">
-        <f t="shared" si="3"/>
         <v>6.0000000000000005E-2</v>
       </c>
       <c r="H8" s="7">
@@ -3074,7 +3060,7 @@
         <v>0.19000000000000003</v>
       </c>
       <c r="I8" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6.0000000000000005E-2</v>
       </c>
       <c r="J8" s="1">
@@ -3084,7 +3070,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -3101,12 +3087,11 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="10">
+        <v>0.72</v>
+      </c>
+      <c r="G9" s="7">
         <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-      <c r="G9" s="7">
-        <f t="shared" si="3"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H9" s="7">
@@ -3114,7 +3099,7 @@
         <v>0.18000000000000002</v>
       </c>
       <c r="I9" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="J9" s="1">
@@ -3124,7 +3109,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -3141,12 +3126,11 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="G10" s="7">
         <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="G10" s="7">
-        <f t="shared" si="3"/>
         <v>0.08</v>
       </c>
       <c r="H10" s="7">
@@ -3154,7 +3138,7 @@
         <v>0.17</v>
       </c>
       <c r="I10" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.08</v>
       </c>
       <c r="J10" s="1">
@@ -3164,7 +3148,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -3181,12 +3165,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="10">
+        <v>0.94</v>
+      </c>
+      <c r="G11" s="7">
         <f t="shared" si="2"/>
-        <v>55</v>
-      </c>
-      <c r="G11" s="7">
-        <f t="shared" si="3"/>
         <v>0.09</v>
       </c>
       <c r="H11" s="7">
@@ -3194,7 +3177,7 @@
         <v>0.16</v>
       </c>
       <c r="I11" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.09</v>
       </c>
       <c r="J11" s="1">
@@ -3204,7 +3187,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -3221,12 +3204,11 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="10">
+        <v>0.69</v>
+      </c>
+      <c r="G12" s="7">
         <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="G12" s="7">
-        <f t="shared" si="3"/>
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="H12" s="7">
@@ -3234,7 +3216,7 @@
         <v>0.15</v>
       </c>
       <c r="I12" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="J12" s="1">
@@ -3244,7 +3226,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -3261,12 +3243,11 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="10">
+        <v>1.04</v>
+      </c>
+      <c r="G13" s="7">
         <f t="shared" si="2"/>
-        <v>65</v>
-      </c>
-      <c r="G13" s="7">
-        <f t="shared" si="3"/>
         <v>0.10999999999999999</v>
       </c>
       <c r="H13" s="7">
@@ -3274,7 +3255,7 @@
         <v>0.13999999999999999</v>
       </c>
       <c r="I13" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.10999999999999999</v>
       </c>
       <c r="J13" s="1">
@@ -3284,7 +3265,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -3301,12 +3282,11 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G14" s="7">
         <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="G14" s="7">
-        <f t="shared" si="3"/>
         <v>0.11999999999999998</v>
       </c>
       <c r="H14" s="7">
@@ -3314,7 +3294,7 @@
         <v>0.12999999999999998</v>
       </c>
       <c r="I14" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.11999999999999998</v>
       </c>
       <c r="J14" s="1">
@@ -3324,7 +3304,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -3341,12 +3321,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="10">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="G15" s="7">
         <f t="shared" si="2"/>
-        <v>75</v>
-      </c>
-      <c r="G15" s="7">
-        <f t="shared" si="3"/>
         <v>0.12999999999999998</v>
       </c>
       <c r="H15" s="7">
@@ -3354,7 +3333,7 @@
         <v>0.11999999999999998</v>
       </c>
       <c r="I15" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.12999999999999998</v>
       </c>
       <c r="J15" s="1">
@@ -3364,7 +3343,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -3381,12 +3360,11 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="10">
+        <v>0.64</v>
+      </c>
+      <c r="G16" s="7">
         <f t="shared" si="2"/>
-        <v>80</v>
-      </c>
-      <c r="G16" s="7">
-        <f t="shared" si="3"/>
         <v>0.13999999999999999</v>
       </c>
       <c r="H16" s="7">
@@ -3394,7 +3372,7 @@
         <v>0.10999999999999999</v>
       </c>
       <c r="I16" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.13999999999999999</v>
       </c>
       <c r="J16" s="1">
@@ -3404,7 +3382,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -3421,12 +3399,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="10">
+        <v>0.43</v>
+      </c>
+      <c r="G17" s="7">
         <f t="shared" si="2"/>
-        <v>85</v>
-      </c>
-      <c r="G17" s="7">
-        <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
       <c r="H17" s="7">
@@ -3434,7 +3411,7 @@
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="I17" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
       <c r="J17" s="1">
@@ -3444,7 +3421,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -3461,12 +3438,11 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="10">
+        <v>0.77</v>
+      </c>
+      <c r="G18" s="7">
         <f t="shared" si="2"/>
-        <v>90</v>
-      </c>
-      <c r="G18" s="7">
-        <f t="shared" si="3"/>
         <v>0.16</v>
       </c>
       <c r="H18" s="7">
@@ -3474,7 +3450,7 @@
         <v>0.09</v>
       </c>
       <c r="I18" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.16</v>
       </c>
       <c r="J18" s="1">
@@ -3484,7 +3460,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -3501,12 +3477,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="10">
+        <v>1.19</v>
+      </c>
+      <c r="G19" s="7">
         <f t="shared" si="2"/>
-        <v>95</v>
-      </c>
-      <c r="G19" s="7">
-        <f t="shared" si="3"/>
         <v>0.17</v>
       </c>
       <c r="H19" s="7">
@@ -3514,7 +3489,7 @@
         <v>0.08</v>
       </c>
       <c r="I19" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.17</v>
       </c>
       <c r="J19" s="1">
@@ -3524,7 +3499,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -3541,12 +3516,11 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="10">
+        <v>2.38</v>
+      </c>
+      <c r="G20" s="7">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="G20" s="7">
-        <f t="shared" si="3"/>
         <v>0.18000000000000002</v>
       </c>
       <c r="H20" s="7">
@@ -3554,7 +3528,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="I20" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.18000000000000002</v>
       </c>
       <c r="J20" s="1">
@@ -3564,7 +3538,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -3581,12 +3555,11 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="10">
+        <v>2.29</v>
+      </c>
+      <c r="G21" s="7">
         <f t="shared" si="2"/>
-        <v>105</v>
-      </c>
-      <c r="G21" s="7">
-        <f t="shared" si="3"/>
         <v>0.19000000000000003</v>
       </c>
       <c r="H21" s="7">
@@ -3594,7 +3567,7 @@
         <v>6.0000000000000005E-2</v>
       </c>
       <c r="I21" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.19000000000000003</v>
       </c>
       <c r="J21" s="2" t="s">
@@ -3604,7 +3577,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -3621,12 +3594,11 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="G22" s="7">
         <f t="shared" si="2"/>
-        <v>110</v>
-      </c>
-      <c r="G22" s="7">
-        <f t="shared" si="3"/>
         <v>0.20000000000000004</v>
       </c>
       <c r="H22" s="7">
@@ -3634,7 +3606,7 @@
         <v>0.05</v>
       </c>
       <c r="I22" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.20000000000000004</v>
       </c>
       <c r="J22" s="1">
@@ -3644,7 +3616,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -3661,12 +3633,11 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="10">
+        <v>0.64</v>
+      </c>
+      <c r="G23" s="7">
         <f t="shared" si="2"/>
-        <v>115</v>
-      </c>
-      <c r="G23" s="7">
-        <f t="shared" si="3"/>
         <v>0.21000000000000005</v>
       </c>
       <c r="H23" s="7">
@@ -3674,7 +3645,7 @@
         <v>0.04</v>
       </c>
       <c r="I23" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.21000000000000005</v>
       </c>
       <c r="J23" s="1">
@@ -3684,7 +3655,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -3701,12 +3672,11 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="10">
+        <v>0.78</v>
+      </c>
+      <c r="G24" s="7">
         <f t="shared" si="2"/>
-        <v>120</v>
-      </c>
-      <c r="G24" s="7">
-        <f t="shared" si="3"/>
         <v>0.22000000000000006</v>
       </c>
       <c r="H24" s="7">
@@ -3714,7 +3684,7 @@
         <v>0.03</v>
       </c>
       <c r="I24" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.22000000000000006</v>
       </c>
       <c r="J24" s="1">
@@ -3724,7 +3694,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -3741,12 +3711,11 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="10">
+        <v>1.77</v>
+      </c>
+      <c r="G25" s="7">
         <f t="shared" si="2"/>
-        <v>125</v>
-      </c>
-      <c r="G25" s="7">
-        <f t="shared" si="3"/>
         <v>0.23000000000000007</v>
       </c>
       <c r="H25" s="7">
@@ -3754,7 +3723,7 @@
         <v>0.02</v>
       </c>
       <c r="I25" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.23000000000000007</v>
       </c>
       <c r="J25" s="1">
@@ -3764,7 +3733,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -3781,12 +3750,11 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="10">
+        <v>0.76</v>
+      </c>
+      <c r="G26" s="7">
         <f t="shared" si="2"/>
-        <v>130</v>
-      </c>
-      <c r="G26" s="7">
-        <f t="shared" si="3"/>
         <v>0.24000000000000007</v>
       </c>
       <c r="H26" s="7">
@@ -3794,7 +3762,7 @@
         <v>0.01</v>
       </c>
       <c r="I26" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.24000000000000007</v>
       </c>
       <c r="J26" s="1">
@@ -3804,11 +3772,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>72</v>
       </c>
@@ -3820,7 +3788,7 @@
       </c>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>75</v>
       </c>
@@ -3828,7 +3796,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>84</v>
       </c>
@@ -3836,7 +3804,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>81</v>
       </c>
@@ -3844,10 +3812,10 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>90</v>
       </c>

</xml_diff>